<commit_message>
removed software and hardware config columns
</commit_message>
<xml_diff>
--- a/experiment_nosql.xlsx
+++ b/experiment_nosql.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\api_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793A520B-7437-4E0B-827B-EB840EDCCBCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2FD162-089B-40C0-BA39-AE0FE8101049}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2985" yWindow="2985" windowWidth="18000" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>id_experimento</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t>cenario</t>
-  </si>
-  <si>
-    <t>configuracao_hard</t>
-  </si>
-  <si>
-    <t>configuracao_soft</t>
   </si>
   <si>
     <t>funcao_api</t>
@@ -410,26 +404,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="N50" sqref="A2:N50"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,12 +455,6 @@
       </c>
       <c r="K1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests 9000 samples
</commit_message>
<xml_diff>
--- a/experiment_nosql.xlsx
+++ b/experiment_nosql.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L301"/>
+  <dimension ref="A1:L304"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
@@ -15521,6 +15521,156 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>2020-10-29 202911235114</t>
+        </is>
+      </c>
+      <c r="C302" s="4" t="n">
+        <v>44133</v>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>21:44:30.509073</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="G302" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H302" t="n">
+        <v>2088000</v>
+      </c>
+      <c r="I302" t="n">
+        <v>9000</v>
+      </c>
+      <c r="J302" s="5" t="n">
+        <v>44133.85360225826</v>
+      </c>
+      <c r="K302" s="5" t="n">
+        <v>44133.90590866943</v>
+      </c>
+      <c r="L302" t="inlineStr">
+        <is>
+          <t>1:15:19.273925</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>2020-10-29 214431754691</t>
+        </is>
+      </c>
+      <c r="C303" s="4" t="n">
+        <v>44133</v>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>22:59:50.912751</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>single client / single read</t>
+        </is>
+      </c>
+      <c r="G303" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H303" t="n">
+        <v>2088000</v>
+      </c>
+      <c r="I303" t="n">
+        <v>9000</v>
+      </c>
+      <c r="J303" s="5" t="n">
+        <v>44133.9059230867</v>
+      </c>
+      <c r="K303" s="5" t="n">
+        <v>44133.95822815644</v>
+      </c>
+      <c r="L303" t="inlineStr">
+        <is>
+          <t>1:15:19.158025</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>2020-10-29 225956218773</t>
+        </is>
+      </c>
+      <c r="C304" s="4" t="n">
+        <v>44134</v>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>00:16:05.817301</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="G304" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H304" t="n">
+        <v>2111200</v>
+      </c>
+      <c r="I304" t="n">
+        <v>9100</v>
+      </c>
+      <c r="J304" s="5" t="n">
+        <v>44133.95828956913</v>
+      </c>
+      <c r="K304" s="5" t="n">
+        <v>44134.01117844055</v>
+      </c>
+      <c r="L304" t="inlineStr">
+        <is>
+          <t>1:16:09.598491</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
added tests flask application
</commit_message>
<xml_diff>
--- a/experiment_nosql.xlsx
+++ b/experiment_nosql.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L304"/>
+  <dimension ref="A1:L386"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
@@ -15671,6 +15671,4106 @@
         </is>
       </c>
     </row>
+    <row r="305">
+      <c r="A305" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>2020-11-01 132107760526</t>
+        </is>
+      </c>
+      <c r="C305" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>13:21:08.297898</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G305" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H305" t="n">
+        <v>23200</v>
+      </c>
+      <c r="I305" t="n">
+        <v>100</v>
+      </c>
+      <c r="J305" s="5" t="n">
+        <v>44136.55633982091</v>
+      </c>
+      <c r="K305" s="5" t="n">
+        <v>44136.5563460402</v>
+      </c>
+      <c r="L305" t="inlineStr">
+        <is>
+          <t>0:00:00.537347</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>2020-11-01 132109677821</t>
+        </is>
+      </c>
+      <c r="C306" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>13:21:10.193854</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H306" t="n">
+        <v>23200</v>
+      </c>
+      <c r="I306" t="n">
+        <v>100</v>
+      </c>
+      <c r="J306" s="5" t="n">
+        <v>44136.55636201182</v>
+      </c>
+      <c r="K306" s="5" t="n">
+        <v>44136.55636798414</v>
+      </c>
+      <c r="L306" t="inlineStr">
+        <is>
+          <t>0:00:00.516009</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>2020-11-01 132342727358</t>
+        </is>
+      </c>
+      <c r="C307" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>13:23:45.408103</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G307" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H307" t="n">
+        <v>116000</v>
+      </c>
+      <c r="I307" t="n">
+        <v>500</v>
+      </c>
+      <c r="J307" s="5" t="n">
+        <v>44136.5581334185</v>
+      </c>
+      <c r="K307" s="5" t="n">
+        <v>44136.55816444528</v>
+      </c>
+      <c r="L307" t="inlineStr">
+        <is>
+          <t>0:00:02.680714</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>2020-11-01 132346664703</t>
+        </is>
+      </c>
+      <c r="C308" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>13:23:49.405419</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G308" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H308" t="n">
+        <v>116000</v>
+      </c>
+      <c r="I308" t="n">
+        <v>500</v>
+      </c>
+      <c r="J308" s="5" t="n">
+        <v>44136.55817898962</v>
+      </c>
+      <c r="K308" s="5" t="n">
+        <v>44136.55821071052</v>
+      </c>
+      <c r="L308" t="inlineStr">
+        <is>
+          <t>0:00:02.740686</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>2020-11-01 132352626954</t>
+        </is>
+      </c>
+      <c r="C309" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>13:23:58.190031</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G309" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H309" t="n">
+        <v>232000</v>
+      </c>
+      <c r="I309" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J309" s="5" t="n">
+        <v>44136.55824799716</v>
+      </c>
+      <c r="K309" s="5" t="n">
+        <v>44136.55831238428</v>
+      </c>
+      <c r="L309" t="inlineStr">
+        <is>
+          <t>0:00:05.563048</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>2020-11-01 132359335197</t>
+        </is>
+      </c>
+      <c r="C310" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>13:24:04.864558</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H310" t="n">
+        <v>232000</v>
+      </c>
+      <c r="I310" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J310" s="5" t="n">
+        <v>44136.55832563886</v>
+      </c>
+      <c r="K310" s="5" t="n">
+        <v>44136.55838963524</v>
+      </c>
+      <c r="L310" t="inlineStr">
+        <is>
+          <t>0:00:05.529288</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>2020-11-01 132408058557</t>
+        </is>
+      </c>
+      <c r="C311" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>13:24:16.245177</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G311" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H311" t="n">
+        <v>348000</v>
+      </c>
+      <c r="I311" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J311" s="5" t="n">
+        <v>44136.55842660367</v>
+      </c>
+      <c r="K311" s="5" t="n">
+        <v>44136.55852135589</v>
+      </c>
+      <c r="L311" t="inlineStr">
+        <is>
+          <t>0:00:08.186592</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>2020-11-01 132417415529</t>
+        </is>
+      </c>
+      <c r="C312" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>13:24:25.598103</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G312" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H312" t="n">
+        <v>348000</v>
+      </c>
+      <c r="I312" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J312" s="5" t="n">
+        <v>44136.55853490195</v>
+      </c>
+      <c r="K312" s="5" t="n">
+        <v>44136.55862960734</v>
+      </c>
+      <c r="L312" t="inlineStr">
+        <is>
+          <t>0:00:08.182545</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>2020-11-01 132428788555</t>
+        </is>
+      </c>
+      <c r="C313" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>13:24:39.804933</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G313" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H313" t="n">
+        <v>464000</v>
+      </c>
+      <c r="I313" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J313" s="5" t="n">
+        <v>44136.5586665342</v>
+      </c>
+      <c r="K313" s="5" t="n">
+        <v>44136.55879403832</v>
+      </c>
+      <c r="L313" t="inlineStr">
+        <is>
+          <t>0:00:11.016356</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>2020-11-01 132440951620</t>
+        </is>
+      </c>
+      <c r="C314" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>13:24:51.910164</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G314" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H314" t="n">
+        <v>464000</v>
+      </c>
+      <c r="I314" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J314" s="5" t="n">
+        <v>44136.55880731043</v>
+      </c>
+      <c r="K314" s="5" t="n">
+        <v>44136.55893414508</v>
+      </c>
+      <c r="L314" t="inlineStr">
+        <is>
+          <t>0:00:10.958515</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>2020-11-01 132455143490</t>
+        </is>
+      </c>
+      <c r="C315" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>13:25:08.962246</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G315" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H315" t="n">
+        <v>580000</v>
+      </c>
+      <c r="I315" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J315" s="5" t="n">
+        <v>44136.55897156817</v>
+      </c>
+      <c r="K315" s="5" t="n">
+        <v>44136.55913150717</v>
+      </c>
+      <c r="L315" t="inlineStr">
+        <is>
+          <t>0:00:13.818730</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>2020-11-01 132510104855</t>
+        </is>
+      </c>
+      <c r="C316" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>13:25:23.835576</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G316" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H316" t="n">
+        <v>580000</v>
+      </c>
+      <c r="I316" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J316" s="5" t="n">
+        <v>44136.55914473212</v>
+      </c>
+      <c r="K316" s="5" t="n">
+        <v>44136.55930365219</v>
+      </c>
+      <c r="L316" t="inlineStr">
+        <is>
+          <t>0:00:13.730693</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>2020-11-01 132527040960</t>
+        </is>
+      </c>
+      <c r="C317" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>13:25:43.637155</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G317" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H317" t="n">
+        <v>696000</v>
+      </c>
+      <c r="I317" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J317" s="5" t="n">
+        <v>44136.55934075185</v>
+      </c>
+      <c r="K317" s="5" t="n">
+        <v>44136.55953283714</v>
+      </c>
+      <c r="L317" t="inlineStr">
+        <is>
+          <t>0:00:16.596169</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>2020-11-01 132544814598</t>
+        </is>
+      </c>
+      <c r="C318" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>13:26:01.360421</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G318" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H318" t="n">
+        <v>696000</v>
+      </c>
+      <c r="I318" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J318" s="5" t="n">
+        <v>44136.55954646526</v>
+      </c>
+      <c r="K318" s="5" t="n">
+        <v>44136.55973796754</v>
+      </c>
+      <c r="L318" t="inlineStr">
+        <is>
+          <t>0:00:16.545797</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>2020-11-01 132604565908</t>
+        </is>
+      </c>
+      <c r="C319" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>13:26:24.118838</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G319" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H319" t="n">
+        <v>812000</v>
+      </c>
+      <c r="I319" t="n">
+        <v>3500</v>
+      </c>
+      <c r="J319" s="5" t="n">
+        <v>44136.55977506838</v>
+      </c>
+      <c r="K319" s="5" t="n">
+        <v>44136.56000137512</v>
+      </c>
+      <c r="L319" t="inlineStr">
+        <is>
+          <t>0:00:19.552902</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>2020-11-01 132625291036</t>
+        </is>
+      </c>
+      <c r="C320" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>13:26:44.627649</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G320" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H320" t="n">
+        <v>812000</v>
+      </c>
+      <c r="I320" t="n">
+        <v>3500</v>
+      </c>
+      <c r="J320" s="5" t="n">
+        <v>44136.56001494254</v>
+      </c>
+      <c r="K320" s="5" t="n">
+        <v>44136.5602387455</v>
+      </c>
+      <c r="L320" t="inlineStr">
+        <is>
+          <t>0:00:19.336575</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>2020-11-01 132647869985</t>
+        </is>
+      </c>
+      <c r="C321" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>13:27:09.959852</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G321" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H321" t="n">
+        <v>928000</v>
+      </c>
+      <c r="I321" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J321" s="5" t="n">
+        <v>44136.56027627298</v>
+      </c>
+      <c r="K321" s="5" t="n">
+        <v>44136.56053194241</v>
+      </c>
+      <c r="L321" t="inlineStr">
+        <is>
+          <t>0:00:22.089839</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>2020-11-01 132711113824</t>
+        </is>
+      </c>
+      <c r="C322" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>13:27:33.121743</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G322" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H322" t="n">
+        <v>928000</v>
+      </c>
+      <c r="I322" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J322" s="5" t="n">
+        <v>44136.56054529889</v>
+      </c>
+      <c r="K322" s="5" t="n">
+        <v>44136.56080001979</v>
+      </c>
+      <c r="L322" t="inlineStr">
+        <is>
+          <t>0:00:22.007887</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>2020-11-01 132736344394</t>
+        </is>
+      </c>
+      <c r="C323" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>13:28:01.282888</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G323" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H323" t="n">
+        <v>1044000</v>
+      </c>
+      <c r="I323" t="n">
+        <v>4500</v>
+      </c>
+      <c r="J323" s="5" t="n">
+        <v>44136.56083731939</v>
+      </c>
+      <c r="K323" s="5" t="n">
+        <v>44136.56112595903</v>
+      </c>
+      <c r="L323" t="inlineStr">
+        <is>
+          <t>0:00:24.938465</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>2020-11-01 132802458836</t>
+        </is>
+      </c>
+      <c r="C324" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>13:28:27.240542</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G324" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H324" t="n">
+        <v>1044000</v>
+      </c>
+      <c r="I324" t="n">
+        <v>4500</v>
+      </c>
+      <c r="J324" s="5" t="n">
+        <v>44136.56113956986</v>
+      </c>
+      <c r="K324" s="5" t="n">
+        <v>44136.56142639486</v>
+      </c>
+      <c r="L324" t="inlineStr">
+        <is>
+          <t>0:00:24.781680</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>2020-11-01 132830454526</t>
+        </is>
+      </c>
+      <c r="C325" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>13:28:58.113692</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G325" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H325" t="n">
+        <v>1160000</v>
+      </c>
+      <c r="I325" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J325" s="5" t="n">
+        <v>44136.56146359405</v>
+      </c>
+      <c r="K325" s="5" t="n">
+        <v>44136.56178372295</v>
+      </c>
+      <c r="L325" t="inlineStr">
+        <is>
+          <t>0:00:27.659137</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>2020-11-01 132859271176</t>
+        </is>
+      </c>
+      <c r="C326" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>13:29:26.826464</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G326" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H326" t="n">
+        <v>1160000</v>
+      </c>
+      <c r="I326" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J326" s="5" t="n">
+        <v>44136.56179712009</v>
+      </c>
+      <c r="K326" s="5" t="n">
+        <v>44136.56211604673</v>
+      </c>
+      <c r="L326" t="inlineStr">
+        <is>
+          <t>0:00:27.555261</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>2020-11-01 132930078385</t>
+        </is>
+      </c>
+      <c r="C327" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>13:30:00.517710</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G327" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H327" t="n">
+        <v>1276000</v>
+      </c>
+      <c r="I327" t="n">
+        <v>5500</v>
+      </c>
+      <c r="J327" s="5" t="n">
+        <v>44136.56215368501</v>
+      </c>
+      <c r="K327" s="5" t="n">
+        <v>44136.5625059917</v>
+      </c>
+      <c r="L327" t="inlineStr">
+        <is>
+          <t>0:00:30.439298</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>2020-11-01 133001663974</t>
+        </is>
+      </c>
+      <c r="C328" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>13:30:31.975866</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G328" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H328" t="n">
+        <v>1276000</v>
+      </c>
+      <c r="I328" t="n">
+        <v>5500</v>
+      </c>
+      <c r="J328" s="5" t="n">
+        <v>44136.56251925896</v>
+      </c>
+      <c r="K328" s="5" t="n">
+        <v>44136.56287009074</v>
+      </c>
+      <c r="L328" t="inlineStr">
+        <is>
+          <t>0:00:30.311866</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>2020-11-01 133035213820</t>
+        </is>
+      </c>
+      <c r="C329" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>13:31:08.355559</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G329" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H329" t="n">
+        <v>1392000</v>
+      </c>
+      <c r="I329" t="n">
+        <v>6000</v>
+      </c>
+      <c r="J329" s="5" t="n">
+        <v>44136.56290756736</v>
+      </c>
+      <c r="K329" s="5" t="n">
+        <v>44136.56329115202</v>
+      </c>
+      <c r="L329" t="inlineStr">
+        <is>
+          <t>0:00:33.141714</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>2020-11-01 133109535179</t>
+        </is>
+      </c>
+      <c r="C330" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>13:31:42.610123</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G330" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H330" t="n">
+        <v>1392000</v>
+      </c>
+      <c r="I330" t="n">
+        <v>6000</v>
+      </c>
+      <c r="J330" s="5" t="n">
+        <v>44136.56330480531</v>
+      </c>
+      <c r="K330" s="5" t="n">
+        <v>44136.56368761683</v>
+      </c>
+      <c r="L330" t="inlineStr">
+        <is>
+          <t>0:00:33.074915</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>2020-11-01 133145843271</t>
+        </is>
+      </c>
+      <c r="C331" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>13:32:21.767066</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G331" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H331" t="n">
+        <v>1508000</v>
+      </c>
+      <c r="I331" t="n">
+        <v>6500</v>
+      </c>
+      <c r="J331" s="5" t="n">
+        <v>44136.56372503786</v>
+      </c>
+      <c r="K331" s="5" t="n">
+        <v>44136.56414082224</v>
+      </c>
+      <c r="L331" t="inlineStr">
+        <is>
+          <t>0:00:35.923771</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>2020-11-01 133222918946</t>
+        </is>
+      </c>
+      <c r="C332" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>13:32:58.769727</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G332" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H332" t="n">
+        <v>1508000</v>
+      </c>
+      <c r="I332" t="n">
+        <v>6500</v>
+      </c>
+      <c r="J332" s="5" t="n">
+        <v>44136.56415415447</v>
+      </c>
+      <c r="K332" s="5" t="n">
+        <v>44136.56456909372</v>
+      </c>
+      <c r="L332" t="inlineStr">
+        <is>
+          <t>0:00:35.850751</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>2020-11-01 133302032209</t>
+        </is>
+      </c>
+      <c r="C333" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>13:33:40.901410</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G333" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H333" t="n">
+        <v>1624000</v>
+      </c>
+      <c r="I333" t="n">
+        <v>7000</v>
+      </c>
+      <c r="J333" s="5" t="n">
+        <v>44136.56460685427</v>
+      </c>
+      <c r="K333" s="5" t="n">
+        <v>44136.56505672897</v>
+      </c>
+      <c r="L333" t="inlineStr">
+        <is>
+          <t>0:00:38.869174</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>2020-11-01 133342059811</t>
+        </is>
+      </c>
+      <c r="C334" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>13:34:20.841747</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G334" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H334" t="n">
+        <v>1624000</v>
+      </c>
+      <c r="I334" t="n">
+        <v>7000</v>
+      </c>
+      <c r="J334" s="5" t="n">
+        <v>44136.5650701367</v>
+      </c>
+      <c r="K334" s="5" t="n">
+        <v>44136.56551900136</v>
+      </c>
+      <c r="L334" t="inlineStr">
+        <is>
+          <t>0:00:38.781906</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>2020-11-01 133424072991</t>
+        </is>
+      </c>
+      <c r="C335" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>13:35:05.522317</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G335" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H335" t="n">
+        <v>1740000</v>
+      </c>
+      <c r="I335" t="n">
+        <v>7500</v>
+      </c>
+      <c r="J335" s="5" t="n">
+        <v>44136.56555640036</v>
+      </c>
+      <c r="K335" s="5" t="n">
+        <v>44136.56603613764</v>
+      </c>
+      <c r="L335" t="inlineStr">
+        <is>
+          <t>0:00:41.449301</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>2020-11-01 133506702316</t>
+        </is>
+      </c>
+      <c r="C336" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>13:35:48.095279</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G336" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H336" t="n">
+        <v>1740000</v>
+      </c>
+      <c r="I336" t="n">
+        <v>7500</v>
+      </c>
+      <c r="J336" s="5" t="n">
+        <v>44136.56604979532</v>
+      </c>
+      <c r="K336" s="5" t="n">
+        <v>44136.56652888023</v>
+      </c>
+      <c r="L336" t="inlineStr">
+        <is>
+          <t>0:00:41.392936</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>2020-11-01 133551346762</t>
+        </is>
+      </c>
+      <c r="C337" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>13:36:35.611889</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F337" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G337" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H337" t="n">
+        <v>1856000</v>
+      </c>
+      <c r="I337" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J337" s="5" t="n">
+        <v>44136.56656651345</v>
+      </c>
+      <c r="K337" s="5" t="n">
+        <v>44136.56707884102</v>
+      </c>
+      <c r="L337" t="inlineStr">
+        <is>
+          <t>0:00:44.265102</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>2020-11-01 133636768492</t>
+        </is>
+      </c>
+      <c r="C338" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>13:37:20.893423</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G338" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H338" t="n">
+        <v>1856000</v>
+      </c>
+      <c r="I338" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J338" s="5" t="n">
+        <v>44136.56709222792</v>
+      </c>
+      <c r="K338" s="5" t="n">
+        <v>44136.5676029328</v>
+      </c>
+      <c r="L338" t="inlineStr">
+        <is>
+          <t>0:00:44.124902</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>2020-11-01 133724169232</t>
+        </is>
+      </c>
+      <c r="C339" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>13:38:11.646023</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G339" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H339" t="n">
+        <v>1972000</v>
+      </c>
+      <c r="I339" t="n">
+        <v>8500</v>
+      </c>
+      <c r="J339" s="5" t="n">
+        <v>44136.56764084759</v>
+      </c>
+      <c r="K339" s="5" t="n">
+        <v>44136.56819034721</v>
+      </c>
+      <c r="L339" t="inlineStr">
+        <is>
+          <t>0:00:47.476767</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>2020-11-01 133812801896</t>
+        </is>
+      </c>
+      <c r="C340" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>13:38:59.860263</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G340" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H340" t="n">
+        <v>1972000</v>
+      </c>
+      <c r="I340" t="n">
+        <v>8500</v>
+      </c>
+      <c r="J340" s="5" t="n">
+        <v>44136.56820372565</v>
+      </c>
+      <c r="K340" s="5" t="n">
+        <v>44136.56874838233</v>
+      </c>
+      <c r="L340" t="inlineStr">
+        <is>
+          <t>0:00:47.058338</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>2020-11-01 133903143652</t>
+        </is>
+      </c>
+      <c r="C341" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>13:39:52.908334</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G341" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H341" t="n">
+        <v>2088000</v>
+      </c>
+      <c r="I341" t="n">
+        <v>9000</v>
+      </c>
+      <c r="J341" s="5" t="n">
+        <v>44136.56878638486</v>
+      </c>
+      <c r="K341" s="5" t="n">
+        <v>44136.56936236464</v>
+      </c>
+      <c r="L341" t="inlineStr">
+        <is>
+          <t>0:00:49.764653</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>2020-11-01 133954079904</t>
+        </is>
+      </c>
+      <c r="C342" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>13:40:43.797813</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G342" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H342" t="n">
+        <v>2088000</v>
+      </c>
+      <c r="I342" t="n">
+        <v>9000</v>
+      </c>
+      <c r="J342" s="5" t="n">
+        <v>44136.56937592482</v>
+      </c>
+      <c r="K342" s="5" t="n">
+        <v>44136.56995136323</v>
+      </c>
+      <c r="L342" t="inlineStr">
+        <is>
+          <t>0:00:49.717879</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>2020-11-01 134047051813</t>
+        </is>
+      </c>
+      <c r="C343" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>13:41:39.489869</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F343" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G343" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H343" t="n">
+        <v>2204000</v>
+      </c>
+      <c r="I343" t="n">
+        <v>9500</v>
+      </c>
+      <c r="J343" s="5" t="n">
+        <v>44136.5699890256</v>
+      </c>
+      <c r="K343" s="5" t="n">
+        <v>44136.57059594721</v>
+      </c>
+      <c r="L343" t="inlineStr">
+        <is>
+          <t>0:00:52.438026</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>2020-11-01 134140680783</t>
+        </is>
+      </c>
+      <c r="C344" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>13:42:33.173795</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F344" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G344" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H344" t="n">
+        <v>2204000</v>
+      </c>
+      <c r="I344" t="n">
+        <v>9500</v>
+      </c>
+      <c r="J344" s="5" t="n">
+        <v>44136.57060973129</v>
+      </c>
+      <c r="K344" s="5" t="n">
+        <v>44136.57121728896</v>
+      </c>
+      <c r="L344" t="inlineStr">
+        <is>
+          <t>0:00:52.492983</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>2020-11-01 134236418729</t>
+        </is>
+      </c>
+      <c r="C345" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>13:43:31.800759</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F345" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G345" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H345" t="n">
+        <v>2320000</v>
+      </c>
+      <c r="I345" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J345" s="5" t="n">
+        <v>44136.5712548464</v>
+      </c>
+      <c r="K345" s="5" t="n">
+        <v>44136.57189584184</v>
+      </c>
+      <c r="L345" t="inlineStr">
+        <is>
+          <t>0:00:55.382006</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>2020-11-01 134332957457</t>
+        </is>
+      </c>
+      <c r="C346" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>13:44:28.330020</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F346" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G346" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H346" t="n">
+        <v>2320000</v>
+      </c>
+      <c r="I346" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J346" s="5" t="n">
+        <v>44136.57190922982</v>
+      </c>
+      <c r="K346" s="5" t="n">
+        <v>44136.57255011566</v>
+      </c>
+      <c r="L346" t="inlineStr">
+        <is>
+          <t>0:00:55.372536</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>2020-11-01 134708183969</t>
+        </is>
+      </c>
+      <c r="C347" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>13:47:19.125942</t>
+        </is>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F347" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G347" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H347" t="n">
+        <v>464000</v>
+      </c>
+      <c r="I347" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J347" s="5" t="n">
+        <v>44136.57440027742</v>
+      </c>
+      <c r="K347" s="5" t="n">
+        <v>44136.5745269203</v>
+      </c>
+      <c r="L347" t="inlineStr">
+        <is>
+          <t>0:00:10.941945</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>2020-11-01 134720394807</t>
+        </is>
+      </c>
+      <c r="C348" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>13:47:31.383362</t>
+        </is>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F348" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G348" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H348" t="n">
+        <v>464000</v>
+      </c>
+      <c r="I348" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J348" s="5" t="n">
+        <v>44136.57454160656</v>
+      </c>
+      <c r="K348" s="5" t="n">
+        <v>44136.57466878862</v>
+      </c>
+      <c r="L348" t="inlineStr">
+        <is>
+          <t>0:00:10.988531</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>2020-11-01 134734631481</t>
+        </is>
+      </c>
+      <c r="C349" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>13:47:56.771660</t>
+        </is>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F349" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G349" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H349" t="n">
+        <v>928000</v>
+      </c>
+      <c r="I349" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J349" s="5" t="n">
+        <v>44136.57470638288</v>
+      </c>
+      <c r="K349" s="5" t="n">
+        <v>44136.57496263463</v>
+      </c>
+      <c r="L349" t="inlineStr">
+        <is>
+          <t>0:00:22.140151</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>2020-11-01 134757934623</t>
+        </is>
+      </c>
+      <c r="C350" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>13:48:19.983751</t>
+        </is>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F350" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G350" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H350" t="n">
+        <v>928000</v>
+      </c>
+      <c r="I350" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J350" s="5" t="n">
+        <v>44136.57497609517</v>
+      </c>
+      <c r="K350" s="5" t="n">
+        <v>44136.5752312931</v>
+      </c>
+      <c r="L350" t="inlineStr">
+        <is>
+          <t>0:00:22.049102</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>2020-11-01 134823213749</t>
+        </is>
+      </c>
+      <c r="C351" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>13:48:56.345527</t>
+        </is>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F351" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G351" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H351" t="n">
+        <v>1392000</v>
+      </c>
+      <c r="I351" t="n">
+        <v>6000</v>
+      </c>
+      <c r="J351" s="5" t="n">
+        <v>44136.57526867765</v>
+      </c>
+      <c r="K351" s="5" t="n">
+        <v>44136.57565214699</v>
+      </c>
+      <c r="L351" t="inlineStr">
+        <is>
+          <t>0:00:33.131751</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>2020-11-01 134857540838</t>
+        </is>
+      </c>
+      <c r="C352" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>13:49:30.700118</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F352" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G352" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H352" t="n">
+        <v>1392000</v>
+      </c>
+      <c r="I352" t="n">
+        <v>6000</v>
+      </c>
+      <c r="J352" s="5" t="n">
+        <v>44136.57566598192</v>
+      </c>
+      <c r="K352" s="5" t="n">
+        <v>44136.57604976958</v>
+      </c>
+      <c r="L352" t="inlineStr">
+        <is>
+          <t>0:00:33.159254</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>2020-11-01 134933935777</t>
+        </is>
+      </c>
+      <c r="C353" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>13:50:18.326350</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F353" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G353" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H353" t="n">
+        <v>1856000</v>
+      </c>
+      <c r="I353" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J353" s="5" t="n">
+        <v>44136.57608721964</v>
+      </c>
+      <c r="K353" s="5" t="n">
+        <v>44136.57660099911</v>
+      </c>
+      <c r="L353" t="inlineStr">
+        <is>
+          <t>0:00:44.390546</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>2020-11-01 135019482360</t>
+        </is>
+      </c>
+      <c r="C354" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>13:51:03.705545</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F354" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G354" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H354" t="n">
+        <v>1856000</v>
+      </c>
+      <c r="I354" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J354" s="5" t="n">
+        <v>44136.57661437917</v>
+      </c>
+      <c r="K354" s="5" t="n">
+        <v>44136.57712622064</v>
+      </c>
+      <c r="L354" t="inlineStr">
+        <is>
+          <t>0:00:44.223102</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>2020-11-01 135106980511</t>
+        </is>
+      </c>
+      <c r="C355" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>13:52:02.824157</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F355" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G355" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H355" t="n">
+        <v>2320000</v>
+      </c>
+      <c r="I355" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J355" s="5" t="n">
+        <v>44136.57716412628</v>
+      </c>
+      <c r="K355" s="5" t="n">
+        <v>44136.57781046447</v>
+      </c>
+      <c r="L355" t="inlineStr">
+        <is>
+          <t>0:00:55.843618</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>2020-11-01 135203983192</t>
+        </is>
+      </c>
+      <c r="C356" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>13:52:59.354783</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H356" t="n">
+        <v>2320000</v>
+      </c>
+      <c r="I356" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J356" s="5" t="n">
+        <v>44136.57782387954</v>
+      </c>
+      <c r="K356" s="5" t="n">
+        <v>44136.57846475395</v>
+      </c>
+      <c r="L356" t="inlineStr">
+        <is>
+          <t>0:00:55.371550</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>2020-11-01 135302653892</t>
+        </is>
+      </c>
+      <c r="C357" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>13:54:09.737372</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F357" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G357" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H357" t="n">
+        <v>2784000</v>
+      </c>
+      <c r="I357" t="n">
+        <v>12000</v>
+      </c>
+      <c r="J357" s="5" t="n">
+        <v>44136.57850293857</v>
+      </c>
+      <c r="K357" s="5" t="n">
+        <v>44136.57927936746</v>
+      </c>
+      <c r="L357" t="inlineStr">
+        <is>
+          <t>0:01:07.083457</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>2020-11-01 135410894722</t>
+        </is>
+      </c>
+      <c r="C358" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>13:55:17.177477</t>
+        </is>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F358" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G358" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H358" t="n">
+        <v>2784000</v>
+      </c>
+      <c r="I358" t="n">
+        <v>12000</v>
+      </c>
+      <c r="J358" s="5" t="n">
+        <v>44136.57929276299</v>
+      </c>
+      <c r="K358" s="5" t="n">
+        <v>44136.5800599242</v>
+      </c>
+      <c r="L358" t="inlineStr">
+        <is>
+          <t>0:01:06.282729</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>2020-11-01 135520459463</t>
+        </is>
+      </c>
+      <c r="C359" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>13:56:38.096429</t>
+        </is>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F359" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G359" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H359" t="n">
+        <v>3248000</v>
+      </c>
+      <c r="I359" t="n">
+        <v>14000</v>
+      </c>
+      <c r="J359" s="5" t="n">
+        <v>44136.58009791045</v>
+      </c>
+      <c r="K359" s="5" t="n">
+        <v>44136.58099648613</v>
+      </c>
+      <c r="L359" t="inlineStr">
+        <is>
+          <t>0:01:17.636938</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>2020-11-01 135639288216</t>
+        </is>
+      </c>
+      <c r="C360" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>13:57:56.683117</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F360" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G360" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H360" t="n">
+        <v>3248000</v>
+      </c>
+      <c r="I360" t="n">
+        <v>14000</v>
+      </c>
+      <c r="J360" s="5" t="n">
+        <v>44136.58101028028</v>
+      </c>
+      <c r="K360" s="5" t="n">
+        <v>44136.58190605429</v>
+      </c>
+      <c r="L360" t="inlineStr">
+        <is>
+          <t>0:01:17.394875</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>2020-11-01 135759958149</t>
+        </is>
+      </c>
+      <c r="C361" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>13:59:28.598589</t>
+        </is>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F361" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G361" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H361" t="n">
+        <v>3712000</v>
+      </c>
+      <c r="I361" t="n">
+        <v>16000</v>
+      </c>
+      <c r="J361" s="5" t="n">
+        <v>44136.58194396006</v>
+      </c>
+      <c r="K361" s="5" t="n">
+        <v>44136.58296989075</v>
+      </c>
+      <c r="L361" t="inlineStr">
+        <is>
+          <t>0:01:28.640412</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>2020-11-01 135929792445</t>
+        </is>
+      </c>
+      <c r="C362" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>14:00:58.205573</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F362" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G362" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H362" t="n">
+        <v>3712000</v>
+      </c>
+      <c r="I362" t="n">
+        <v>16000</v>
+      </c>
+      <c r="J362" s="5" t="n">
+        <v>44136.58298370885</v>
+      </c>
+      <c r="K362" s="5" t="n">
+        <v>44136.58400700862</v>
+      </c>
+      <c r="L362" t="inlineStr">
+        <is>
+          <t>0:01:28.413101</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>2020-11-01 140101510801</t>
+        </is>
+      </c>
+      <c r="C363" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>14:02:41.297647</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G363" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H363" t="n">
+        <v>4176000</v>
+      </c>
+      <c r="I363" t="n">
+        <v>18000</v>
+      </c>
+      <c r="J363" s="5" t="n">
+        <v>44136.5840452639</v>
+      </c>
+      <c r="K363" s="5" t="n">
+        <v>44136.58520020393</v>
+      </c>
+      <c r="L363" t="inlineStr">
+        <is>
+          <t>0:01:39.786819</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>2020-11-01 140242465907</t>
+        </is>
+      </c>
+      <c r="C364" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>14:04:22.788023</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G364" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H364" t="n">
+        <v>4176000</v>
+      </c>
+      <c r="I364" t="n">
+        <v>18000</v>
+      </c>
+      <c r="J364" s="5" t="n">
+        <v>44136.58521372579</v>
+      </c>
+      <c r="K364" s="5" t="n">
+        <v>44136.5863748611</v>
+      </c>
+      <c r="L364" t="inlineStr">
+        <is>
+          <t>0:01:40.322092</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>2020-11-01 140426138148</t>
+        </is>
+      </c>
+      <c r="C365" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>14:06:16.942217</t>
+        </is>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F365" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G365" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H365" t="n">
+        <v>4640000</v>
+      </c>
+      <c r="I365" t="n">
+        <v>20000</v>
+      </c>
+      <c r="J365" s="5" t="n">
+        <v>44136.58641363597</v>
+      </c>
+      <c r="K365" s="5" t="n">
+        <v>44136.58769609017</v>
+      </c>
+      <c r="L365" t="inlineStr">
+        <is>
+          <t>0:01:50.804043</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>2020-11-01 140618114372</t>
+        </is>
+      </c>
+      <c r="C366" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>14:08:08.986244</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F366" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G366" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H366" t="n">
+        <v>4640000</v>
+      </c>
+      <c r="I366" t="n">
+        <v>20000</v>
+      </c>
+      <c r="J366" s="5" t="n">
+        <v>44136.58770965707</v>
+      </c>
+      <c r="K366" s="5" t="n">
+        <v>44136.58899289527</v>
+      </c>
+      <c r="L366" t="inlineStr">
+        <is>
+          <t>0:01:50.871780</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>2020-11-01 140812345281</t>
+        </is>
+      </c>
+      <c r="C367" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>14:10:14.266250</t>
+        </is>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F367" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G367" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H367" t="n">
+        <v>5104000</v>
+      </c>
+      <c r="I367" t="n">
+        <v>22000</v>
+      </c>
+      <c r="J367" s="5" t="n">
+        <v>44136.5890317741</v>
+      </c>
+      <c r="K367" s="5" t="n">
+        <v>44136.59044289603</v>
+      </c>
+      <c r="L367" t="inlineStr">
+        <is>
+          <t>0:02:01.920936</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>2020-11-01 141015439391</t>
+        </is>
+      </c>
+      <c r="C368" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>14:12:17.254435</t>
+        </is>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F368" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G368" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H368" t="n">
+        <v>5104000</v>
+      </c>
+      <c r="I368" t="n">
+        <v>22000</v>
+      </c>
+      <c r="J368" s="5" t="n">
+        <v>44136.59045647442</v>
+      </c>
+      <c r="K368" s="5" t="n">
+        <v>44136.59186637047</v>
+      </c>
+      <c r="L368" t="inlineStr">
+        <is>
+          <t>0:02:01.815018</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>2020-11-01 141220598497</t>
+        </is>
+      </c>
+      <c r="C369" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>14:14:34.102337</t>
+        </is>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F369" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G369" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H369" t="n">
+        <v>5568000</v>
+      </c>
+      <c r="I369" t="n">
+        <v>24000</v>
+      </c>
+      <c r="J369" s="5" t="n">
+        <v>44136.5919050752</v>
+      </c>
+      <c r="K369" s="5" t="n">
+        <v>44136.59345025823</v>
+      </c>
+      <c r="L369" t="inlineStr">
+        <is>
+          <t>0:02:13.503814</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>2020-11-01 141435303282</t>
+        </is>
+      </c>
+      <c r="C370" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>14:16:48.047489</t>
+        </is>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F370" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G370" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H370" t="n">
+        <v>5568000</v>
+      </c>
+      <c r="I370" t="n">
+        <v>24000</v>
+      </c>
+      <c r="J370" s="5" t="n">
+        <v>44136.59346415836</v>
+      </c>
+      <c r="K370" s="5" t="n">
+        <v>44136.59500054935</v>
+      </c>
+      <c r="L370" t="inlineStr">
+        <is>
+          <t>0:02:12.744182</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>2020-11-01 141651408184</t>
+        </is>
+      </c>
+      <c r="C371" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>14:19:15.608639</t>
+        </is>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F371" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G371" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H371" t="n">
+        <v>6032000</v>
+      </c>
+      <c r="I371" t="n">
+        <v>26000</v>
+      </c>
+      <c r="J371" s="5" t="n">
+        <v>44136.59503944658</v>
+      </c>
+      <c r="K371" s="5" t="n">
+        <v>44136.59670843299</v>
+      </c>
+      <c r="L371" t="inlineStr">
+        <is>
+          <t>0:02:24.200426</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>2020-11-01 141916809425</t>
+        </is>
+      </c>
+      <c r="C372" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>14:21:40.378567</t>
+        </is>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F372" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G372" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H372" t="n">
+        <v>6032000</v>
+      </c>
+      <c r="I372" t="n">
+        <v>26000</v>
+      </c>
+      <c r="J372" s="5" t="n">
+        <v>44136.59672233131</v>
+      </c>
+      <c r="K372" s="5" t="n">
+        <v>44136.59838401014</v>
+      </c>
+      <c r="L372" t="inlineStr">
+        <is>
+          <t>0:02:23.569051</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>2020-11-01 142143738327</t>
+        </is>
+      </c>
+      <c r="C373" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>14:24:18.933229</t>
+        </is>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F373" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G373" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H373" t="n">
+        <v>6496000</v>
+      </c>
+      <c r="I373" t="n">
+        <v>28000</v>
+      </c>
+      <c r="J373" s="5" t="n">
+        <v>44136.5984228973</v>
+      </c>
+      <c r="K373" s="5" t="n">
+        <v>44136.60021913425</v>
+      </c>
+      <c r="L373" t="inlineStr">
+        <is>
+          <t>0:02:35.194872</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>2020-11-01 142420108227</t>
+        </is>
+      </c>
+      <c r="C374" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>14:26:55.024000</t>
+        </is>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F374" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G374" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H374" t="n">
+        <v>6496000</v>
+      </c>
+      <c r="I374" t="n">
+        <v>28000</v>
+      </c>
+      <c r="J374" s="5" t="n">
+        <v>44136.60023273411</v>
+      </c>
+      <c r="K374" s="5" t="n">
+        <v>44136.60202574043</v>
+      </c>
+      <c r="L374" t="inlineStr">
+        <is>
+          <t>0:02:34.915746</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>2020-11-01 142658434522</t>
+        </is>
+      </c>
+      <c r="C375" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>14:29:44.883806</t>
+        </is>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F375" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G375" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H375" t="n">
+        <v>6960000</v>
+      </c>
+      <c r="I375" t="n">
+        <v>30000</v>
+      </c>
+      <c r="J375" s="5" t="n">
+        <v>44136.60206521438</v>
+      </c>
+      <c r="K375" s="5" t="n">
+        <v>44136.60399171039</v>
+      </c>
+      <c r="L375" t="inlineStr">
+        <is>
+          <t>0:02:46.449256</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>2020-11-01 142946056125</t>
+        </is>
+      </c>
+      <c r="C376" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>14:32:31.916233</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F376" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G376" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H376" t="n">
+        <v>6960000</v>
+      </c>
+      <c r="I376" t="n">
+        <v>30000</v>
+      </c>
+      <c r="J376" s="5" t="n">
+        <v>44136.60400527922</v>
+      </c>
+      <c r="K376" s="5" t="n">
+        <v>44136.6059249561</v>
+      </c>
+      <c r="L376" t="inlineStr">
+        <is>
+          <t>0:02:45.860082</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>2020-11-01 143235341777</t>
+        </is>
+      </c>
+      <c r="C377" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>14:35:32.807357</t>
+        </is>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F377" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G377" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H377" t="n">
+        <v>7424000</v>
+      </c>
+      <c r="I377" t="n">
+        <v>32000</v>
+      </c>
+      <c r="J377" s="5" t="n">
+        <v>44136.6059646039</v>
+      </c>
+      <c r="K377" s="5" t="n">
+        <v>44136.60801860338</v>
+      </c>
+      <c r="L377" t="inlineStr">
+        <is>
+          <t>0:02:57.465555</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>2020-11-01 143533983375</t>
+        </is>
+      </c>
+      <c r="C378" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>14:38:31.530057</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F378" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G378" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H378" t="n">
+        <v>7424000</v>
+      </c>
+      <c r="I378" t="n">
+        <v>32000</v>
+      </c>
+      <c r="J378" s="5" t="n">
+        <v>44136.60803221499</v>
+      </c>
+      <c r="K378" s="5" t="n">
+        <v>44136.61008715312</v>
+      </c>
+      <c r="L378" t="inlineStr">
+        <is>
+          <t>0:02:57.546655</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>2020-11-01 143834954895</t>
+        </is>
+      </c>
+      <c r="C379" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>14:41:44.379849</t>
+        </is>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F379" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G379" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H379" t="n">
+        <v>7888000</v>
+      </c>
+      <c r="I379" t="n">
+        <v>34000</v>
+      </c>
+      <c r="J379" s="5" t="n">
+        <v>44136.61012679278</v>
+      </c>
+      <c r="K379" s="5" t="n">
+        <v>44136.61231921086</v>
+      </c>
+      <c r="L379" t="inlineStr">
+        <is>
+          <t>0:03:09.424923</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>2020-11-01 144145586452</t>
+        </is>
+      </c>
+      <c r="C380" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>14:44:54.791670</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F380" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G380" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H380" t="n">
+        <v>7888000</v>
+      </c>
+      <c r="I380" t="n">
+        <v>34000</v>
+      </c>
+      <c r="J380" s="5" t="n">
+        <v>44136.61233317653</v>
+      </c>
+      <c r="K380" s="5" t="n">
+        <v>44136.61452305136</v>
+      </c>
+      <c r="L380" t="inlineStr">
+        <is>
+          <t>0:03:09.205186</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>2020-11-01 144458226275</t>
+        </is>
+      </c>
+      <c r="C381" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>14:48:18.027021</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F381" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G381" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H381" t="n">
+        <v>8352000</v>
+      </c>
+      <c r="I381" t="n">
+        <v>36000</v>
+      </c>
+      <c r="J381" s="5" t="n">
+        <v>44136.61456280411</v>
+      </c>
+      <c r="K381" s="5" t="n">
+        <v>44136.61687531239</v>
+      </c>
+      <c r="L381" t="inlineStr">
+        <is>
+          <t>0:03:19.800716</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>2020-11-01 144819231618</t>
+        </is>
+      </c>
+      <c r="C382" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>14:51:38.447573</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F382" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G382" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H382" t="n">
+        <v>8352000</v>
+      </c>
+      <c r="I382" t="n">
+        <v>36000</v>
+      </c>
+      <c r="J382" s="5" t="n">
+        <v>44136.61688925484</v>
+      </c>
+      <c r="K382" s="5" t="n">
+        <v>44136.61919499475</v>
+      </c>
+      <c r="L382" t="inlineStr">
+        <is>
+          <t>0:03:19.215929</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>2020-11-01 145141883427</t>
+        </is>
+      </c>
+      <c r="C383" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>14:55:12.624297</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G383" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H383" t="n">
+        <v>8816000</v>
+      </c>
+      <c r="I383" t="n">
+        <v>38000</v>
+      </c>
+      <c r="J383" s="5" t="n">
+        <v>44136.6192347619</v>
+      </c>
+      <c r="K383" s="5" t="n">
+        <v>44136.62167389201</v>
+      </c>
+      <c r="L383" t="inlineStr">
+        <is>
+          <t>0:03:30.740843</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>2020-11-01 145513797849</t>
+        </is>
+      </c>
+      <c r="C384" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>14:58:43.933980</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F384" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G384" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H384" t="n">
+        <v>8816000</v>
+      </c>
+      <c r="I384" t="n">
+        <v>38000</v>
+      </c>
+      <c r="J384" s="5" t="n">
+        <v>44136.62168747509</v>
+      </c>
+      <c r="K384" s="5" t="n">
+        <v>44136.62411960532</v>
+      </c>
+      <c r="L384" t="inlineStr">
+        <is>
+          <t>0:03:30.136051</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>2020-11-01 145847413858</t>
+        </is>
+      </c>
+      <c r="C385" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>15:02:29.405517</t>
+        </is>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F385" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G385" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H385" t="n">
+        <v>9280000</v>
+      </c>
+      <c r="I385" t="n">
+        <v>40000</v>
+      </c>
+      <c r="J385" s="5" t="n">
+        <v>44136.62415988262</v>
+      </c>
+      <c r="K385" s="5" t="n">
+        <v>44136.6267292302</v>
+      </c>
+      <c r="L385" t="inlineStr">
+        <is>
+          <t>0:03:41.991631</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>2020-11-01 150230579690</t>
+        </is>
+      </c>
+      <c r="C386" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>15:06:12.987727</t>
+        </is>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F386" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G386" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H386" t="n">
+        <v>9280000</v>
+      </c>
+      <c r="I386" t="n">
+        <v>40000</v>
+      </c>
+      <c r="J386" s="5" t="n">
+        <v>44136.62674282049</v>
+      </c>
+      <c r="K386" s="5" t="n">
+        <v>44136.62931698693</v>
+      </c>
+      <c r="L386" t="inlineStr">
+        <is>
+          <t>0:03:42.407981</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
added tests nosql +- 40x
</commit_message>
<xml_diff>
--- a/experiment_nosql.xlsx
+++ b/experiment_nosql.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L386"/>
+  <dimension ref="A1:L464"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
@@ -19771,6 +19771,3906 @@
         </is>
       </c>
     </row>
+    <row r="387">
+      <c r="A387" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>2020-11-01 151852516839</t>
+        </is>
+      </c>
+      <c r="C387" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>15:19:03.491173</t>
+        </is>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F387" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G387" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H387" t="n">
+        <v>464000</v>
+      </c>
+      <c r="I387" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J387" s="5" t="n">
+        <v>44136.63810783379</v>
+      </c>
+      <c r="K387" s="5" t="n">
+        <v>44136.63823485124</v>
+      </c>
+      <c r="L387" t="inlineStr">
+        <is>
+          <t>0:00:10.974308</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>2020-11-01 151904779632</t>
+        </is>
+      </c>
+      <c r="C388" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>15:19:15.803015</t>
+        </is>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F388" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G388" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H388" t="n">
+        <v>464000</v>
+      </c>
+      <c r="I388" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J388" s="5" t="n">
+        <v>44136.63824976426</v>
+      </c>
+      <c r="K388" s="5" t="n">
+        <v>44136.63837734935</v>
+      </c>
+      <c r="L388" t="inlineStr">
+        <is>
+          <t>0:00:11.023352</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>2020-11-01 151919055533</t>
+        </is>
+      </c>
+      <c r="C389" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>15:19:41.223193</t>
+        </is>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G389" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H389" t="n">
+        <v>928000</v>
+      </c>
+      <c r="I389" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J389" s="5" t="n">
+        <v>44136.63841499461</v>
+      </c>
+      <c r="K389" s="5" t="n">
+        <v>44136.63867156445</v>
+      </c>
+      <c r="L389" t="inlineStr">
+        <is>
+          <t>0:00:22.167635</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>2020-11-01 151942405832</t>
+        </is>
+      </c>
+      <c r="C390" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>15:20:04.582488</t>
+        </is>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G390" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H390" t="n">
+        <v>928000</v>
+      </c>
+      <c r="I390" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J390" s="5" t="n">
+        <v>44136.63868525267</v>
+      </c>
+      <c r="K390" s="5" t="n">
+        <v>44136.63894192662</v>
+      </c>
+      <c r="L390" t="inlineStr">
+        <is>
+          <t>0:00:22.176628</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>2020-11-01 152007861202</t>
+        </is>
+      </c>
+      <c r="C391" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>15:20:41.166047</t>
+        </is>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F391" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G391" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H391" t="n">
+        <v>1392000</v>
+      </c>
+      <c r="I391" t="n">
+        <v>6000</v>
+      </c>
+      <c r="J391" s="5" t="n">
+        <v>44136.63897987501</v>
+      </c>
+      <c r="K391" s="5" t="n">
+        <v>44136.63936534749</v>
+      </c>
+      <c r="L391" t="inlineStr">
+        <is>
+          <t>0:00:33.304821</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>2020-11-01 152042345968</t>
+        </is>
+      </c>
+      <c r="C392" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>15:21:15.699557</t>
+        </is>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F392" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G392" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H392" t="n">
+        <v>1392000</v>
+      </c>
+      <c r="I392" t="n">
+        <v>6000</v>
+      </c>
+      <c r="J392" s="5" t="n">
+        <v>44136.63937900426</v>
+      </c>
+      <c r="K392" s="5" t="n">
+        <v>44136.63976504083</v>
+      </c>
+      <c r="L392" t="inlineStr">
+        <is>
+          <t>0:00:33.353559</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>2020-11-01 152118942636</t>
+        </is>
+      </c>
+      <c r="C393" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>15:22:03.458016</t>
+        </is>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F393" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G393" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H393" t="n">
+        <v>1856000</v>
+      </c>
+      <c r="I393" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J393" s="5" t="n">
+        <v>44136.63980257681</v>
+      </c>
+      <c r="K393" s="5" t="n">
+        <v>44136.64031780076</v>
+      </c>
+      <c r="L393" t="inlineStr">
+        <is>
+          <t>0:00:44.515350</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>2020-11-01 152204661603</t>
+        </is>
+      </c>
+      <c r="C394" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>15:22:49.166390</t>
+        </is>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F394" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G394" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H394" t="n">
+        <v>1856000</v>
+      </c>
+      <c r="I394" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J394" s="5" t="n">
+        <v>44136.64033173152</v>
+      </c>
+      <c r="K394" s="5" t="n">
+        <v>44136.64084683293</v>
+      </c>
+      <c r="L394" t="inlineStr">
+        <is>
+          <t>0:00:44.504762</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>2020-11-01 152252433873</t>
+        </is>
+      </c>
+      <c r="C395" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>15:23:48.124193</t>
+        </is>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F395" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G395" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H395" t="n">
+        <v>2320000</v>
+      </c>
+      <c r="I395" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J395" s="5" t="n">
+        <v>44136.64088465131</v>
+      </c>
+      <c r="K395" s="5" t="n">
+        <v>44136.64152921492</v>
+      </c>
+      <c r="L395" t="inlineStr">
+        <is>
+          <t>0:00:55.690296</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>2020-11-01 152349329284</t>
+        </is>
+      </c>
+      <c r="C396" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>15:24:44.869512</t>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F396" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G396" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H396" t="n">
+        <v>2320000</v>
+      </c>
+      <c r="I396" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J396" s="5" t="n">
+        <v>44136.64154316301</v>
+      </c>
+      <c r="K396" s="5" t="n">
+        <v>44136.64218598939</v>
+      </c>
+      <c r="L396" t="inlineStr">
+        <is>
+          <t>0:00:55.540199</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>2020-11-01 152448143099</t>
+        </is>
+      </c>
+      <c r="C397" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>15:25:54.859865</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H397" t="n">
+        <v>2784000</v>
+      </c>
+      <c r="I397" t="n">
+        <v>12000</v>
+      </c>
+      <c r="J397" s="5" t="n">
+        <v>44136.64222387846</v>
+      </c>
+      <c r="K397" s="5" t="n">
+        <v>44136.64299606273</v>
+      </c>
+      <c r="L397" t="inlineStr">
+        <is>
+          <t>0:01:06.716721</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>2020-11-01 152556077200</t>
+        </is>
+      </c>
+      <c r="C398" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>15:27:02.896834</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F398" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G398" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H398" t="n">
+        <v>2784000</v>
+      </c>
+      <c r="I398" t="n">
+        <v>12000</v>
+      </c>
+      <c r="J398" s="5" t="n">
+        <v>44136.64301015278</v>
+      </c>
+      <c r="K398" s="5" t="n">
+        <v>44136.64378352785</v>
+      </c>
+      <c r="L398" t="inlineStr">
+        <is>
+          <t>0:01:06.819606</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>2020-11-01 152706189711</t>
+        </is>
+      </c>
+      <c r="C399" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>15:28:24.496254</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F399" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H399" t="n">
+        <v>3248000</v>
+      </c>
+      <c r="I399" t="n">
+        <v>14000</v>
+      </c>
+      <c r="J399" s="5" t="n">
+        <v>44136.64382164017</v>
+      </c>
+      <c r="K399" s="5" t="n">
+        <v>44136.64472796558</v>
+      </c>
+      <c r="L399" t="inlineStr">
+        <is>
+          <t>0:01:18.306515</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>2020-11-01 152825678659</t>
+        </is>
+      </c>
+      <c r="C400" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>15:29:43.603815</t>
+        </is>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F400" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G400" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H400" t="n">
+        <v>3248000</v>
+      </c>
+      <c r="I400" t="n">
+        <v>14000</v>
+      </c>
+      <c r="J400" s="5" t="n">
+        <v>44136.64474165114</v>
+      </c>
+      <c r="K400" s="5" t="n">
+        <v>44136.64564356229</v>
+      </c>
+      <c r="L400" t="inlineStr">
+        <is>
+          <t>0:01:17.925124</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>2020-11-01 152946932293</t>
+        </is>
+      </c>
+      <c r="C401" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>15:31:15.898463</t>
+        </is>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F401" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G401" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H401" t="n">
+        <v>3712000</v>
+      </c>
+      <c r="I401" t="n">
+        <v>16000</v>
+      </c>
+      <c r="J401" s="5" t="n">
+        <v>44136.64568208671</v>
+      </c>
+      <c r="K401" s="5" t="n">
+        <v>44136.64671178746</v>
+      </c>
+      <c r="L401" t="inlineStr">
+        <is>
+          <t>0:01:28.966144</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>2020-11-01 153117083317</t>
+        </is>
+      </c>
+      <c r="C402" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>15:32:46.101762</t>
+        </is>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F402" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G402" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H402" t="n">
+        <v>3712000</v>
+      </c>
+      <c r="I402" t="n">
+        <v>16000</v>
+      </c>
+      <c r="J402" s="5" t="n">
+        <v>44136.64672550136</v>
+      </c>
+      <c r="K402" s="5" t="n">
+        <v>44136.64775580712</v>
+      </c>
+      <c r="L402" t="inlineStr">
+        <is>
+          <t>0:01:29.018417</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>2020-11-01 153249442092</t>
+        </is>
+      </c>
+      <c r="C403" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>15:34:29.854046</t>
+        </is>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F403" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G403" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H403" t="n">
+        <v>4176000</v>
+      </c>
+      <c r="I403" t="n">
+        <v>18000</v>
+      </c>
+      <c r="J403" s="5" t="n">
+        <v>44136.64779446866</v>
+      </c>
+      <c r="K403" s="5" t="n">
+        <v>44136.64895664373</v>
+      </c>
+      <c r="L403" t="inlineStr">
+        <is>
+          <t>0:01:40.411926</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>2020-11-01 153431036572</t>
+        </is>
+      </c>
+      <c r="C404" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>15:36:11.048537</t>
+        </is>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F404" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G404" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H404" t="n">
+        <v>4176000</v>
+      </c>
+      <c r="I404" t="n">
+        <v>18000</v>
+      </c>
+      <c r="J404" s="5" t="n">
+        <v>44136.64897033068</v>
+      </c>
+      <c r="K404" s="5" t="n">
+        <v>44136.65012787627</v>
+      </c>
+      <c r="L404" t="inlineStr">
+        <is>
+          <t>0:01:40.011938</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>2020-11-01 153614414518</t>
+        </is>
+      </c>
+      <c r="C405" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>15:38:06.211110</t>
+        </is>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F405" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G405" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H405" t="n">
+        <v>4640000</v>
+      </c>
+      <c r="I405" t="n">
+        <v>20000</v>
+      </c>
+      <c r="J405" s="5" t="n">
+        <v>44136.6501668347</v>
+      </c>
+      <c r="K405" s="5" t="n">
+        <v>44136.65146077643</v>
+      </c>
+      <c r="L405" t="inlineStr">
+        <is>
+          <t>0:01:51.796566</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>2020-11-01 153807401612</t>
+        </is>
+      </c>
+      <c r="C406" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>15:39:58.688613</t>
+        </is>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F406" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G406" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H406" t="n">
+        <v>4640000</v>
+      </c>
+      <c r="I406" t="n">
+        <v>20000</v>
+      </c>
+      <c r="J406" s="5" t="n">
+        <v>44136.65147455569</v>
+      </c>
+      <c r="K406" s="5" t="n">
+        <v>44136.65276259933</v>
+      </c>
+      <c r="L406" t="inlineStr">
+        <is>
+          <t>0:01:51.286970</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>2020-11-01 154002026451</t>
+        </is>
+      </c>
+      <c r="C407" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>15:42:04.493150</t>
+        </is>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F407" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G407" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H407" t="n">
+        <v>5104000</v>
+      </c>
+      <c r="I407" t="n">
+        <v>22000</v>
+      </c>
+      <c r="J407" s="5" t="n">
+        <v>44136.65280123207</v>
+      </c>
+      <c r="K407" s="5" t="n">
+        <v>44136.65421867037</v>
+      </c>
+      <c r="L407" t="inlineStr">
+        <is>
+          <t>0:02:02.466669</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>2020-11-01 154205711008</t>
+        </is>
+      </c>
+      <c r="C408" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>15:44:08.116071</t>
+        </is>
+      </c>
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F408" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G408" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H408" t="n">
+        <v>5104000</v>
+      </c>
+      <c r="I408" t="n">
+        <v>22000</v>
+      </c>
+      <c r="J408" s="5" t="n">
+        <v>44136.6542327663</v>
+      </c>
+      <c r="K408" s="5" t="n">
+        <v>44136.65564949069</v>
+      </c>
+      <c r="L408" t="inlineStr">
+        <is>
+          <t>0:02:02.404988</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>2020-11-01 154411466457</t>
+        </is>
+      </c>
+      <c r="C409" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>15:46:24.907463</t>
+        </is>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F409" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G409" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H409" t="n">
+        <v>5568000</v>
+      </c>
+      <c r="I409" t="n">
+        <v>24000</v>
+      </c>
+      <c r="J409" s="5" t="n">
+        <v>44136.65568826918</v>
+      </c>
+      <c r="K409" s="5" t="n">
+        <v>44136.65723272497</v>
+      </c>
+      <c r="L409" t="inlineStr">
+        <is>
+          <t>0:02:13.440980</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>2020-11-01 154626125152</t>
+        </is>
+      </c>
+      <c r="C410" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>15:48:39.683214</t>
+        </is>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F410" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G410" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H410" t="n">
+        <v>5568000</v>
+      </c>
+      <c r="I410" t="n">
+        <v>24000</v>
+      </c>
+      <c r="J410" s="5" t="n">
+        <v>44136.65724681889</v>
+      </c>
+      <c r="K410" s="5" t="n">
+        <v>44136.65879262943</v>
+      </c>
+      <c r="L410" t="inlineStr">
+        <is>
+          <t>0:02:13.558031</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>2020-11-01 154843071748</t>
+        </is>
+      </c>
+      <c r="C411" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>15:51:07.853473</t>
+        </is>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F411" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G411" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H411" t="n">
+        <v>6032000</v>
+      </c>
+      <c r="I411" t="n">
+        <v>26000</v>
+      </c>
+      <c r="J411" s="5" t="n">
+        <v>44136.65883184894</v>
+      </c>
+      <c r="K411" s="5" t="n">
+        <v>44136.66050756304</v>
+      </c>
+      <c r="L411" t="inlineStr">
+        <is>
+          <t>0:02:24.781699</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>2020-11-01 155109073186</t>
+        </is>
+      </c>
+      <c r="C412" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>15:53:34.558474</t>
+        </is>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F412" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G412" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H412" t="n">
+        <v>6032000</v>
+      </c>
+      <c r="I412" t="n">
+        <v>26000</v>
+      </c>
+      <c r="J412" s="5" t="n">
+        <v>44136.66052168038</v>
+      </c>
+      <c r="K412" s="5" t="n">
+        <v>44136.66220553761</v>
+      </c>
+      <c r="L412" t="inlineStr">
+        <is>
+          <t>0:02:25.485263</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>2020-11-01 155337945273</t>
+        </is>
+      </c>
+      <c r="C413" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>15:56:13.860346</t>
+        </is>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F413" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G413" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H413" t="n">
+        <v>6496000</v>
+      </c>
+      <c r="I413" t="n">
+        <v>28000</v>
+      </c>
+      <c r="J413" s="5" t="n">
+        <v>44136.66224473696</v>
+      </c>
+      <c r="K413" s="5" t="n">
+        <v>44136.66404930926</v>
+      </c>
+      <c r="L413" t="inlineStr">
+        <is>
+          <t>0:02:35.915047</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>2020-11-01 155615081203</t>
+        </is>
+      </c>
+      <c r="C414" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>15:58:50.802775</t>
+        </is>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F414" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G414" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H414" t="n">
+        <v>6496000</v>
+      </c>
+      <c r="I414" t="n">
+        <v>28000</v>
+      </c>
+      <c r="J414" s="5" t="n">
+        <v>44136.66406343985</v>
+      </c>
+      <c r="K414" s="5" t="n">
+        <v>44136.66586577257</v>
+      </c>
+      <c r="L414" t="inlineStr">
+        <is>
+          <t>0:02:35.721547</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>2020-11-01 155854206801</t>
+        </is>
+      </c>
+      <c r="C415" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>16:01:41.186069</t>
+        </is>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F415" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G415" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H415" t="n">
+        <v>6960000</v>
+      </c>
+      <c r="I415" t="n">
+        <v>30000</v>
+      </c>
+      <c r="J415" s="5" t="n">
+        <v>44136.66590517131</v>
+      </c>
+      <c r="K415" s="5" t="n">
+        <v>44136.66783780139</v>
+      </c>
+      <c r="L415" t="inlineStr">
+        <is>
+          <t>0:02:46.979239</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>2020-11-01 160142412644</t>
+        </is>
+      </c>
+      <c r="C416" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>16:04:29.403579</t>
+        </is>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F416" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G416" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H416" t="n">
+        <v>6960000</v>
+      </c>
+      <c r="I416" t="n">
+        <v>30000</v>
+      </c>
+      <c r="J416" s="5" t="n">
+        <v>44136.66785199818</v>
+      </c>
+      <c r="K416" s="5" t="n">
+        <v>44136.66978476333</v>
+      </c>
+      <c r="L416" t="inlineStr">
+        <is>
+          <t>0:02:46.990908</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>2020-11-01 160432811421</t>
+        </is>
+      </c>
+      <c r="C417" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>16:07:31.610663</t>
+        </is>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F417" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G417" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H417" t="n">
+        <v>7424000</v>
+      </c>
+      <c r="I417" t="n">
+        <v>32000</v>
+      </c>
+      <c r="J417" s="5" t="n">
+        <v>44136.66982420626</v>
+      </c>
+      <c r="K417" s="5" t="n">
+        <v>44136.67189364162</v>
+      </c>
+      <c r="L417" t="inlineStr">
+        <is>
+          <t>0:02:58.799215</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>2020-11-01 160732803708</t>
+        </is>
+      </c>
+      <c r="C418" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>16:10:31.151782</t>
+        </is>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F418" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G418" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H418" t="n">
+        <v>7424000</v>
+      </c>
+      <c r="I418" t="n">
+        <v>32000</v>
+      </c>
+      <c r="J418" s="5" t="n">
+        <v>44136.67190745033</v>
+      </c>
+      <c r="K418" s="5" t="n">
+        <v>44136.67397166382</v>
+      </c>
+      <c r="L418" t="inlineStr">
+        <is>
+          <t>0:02:58.348046</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>2020-11-01 161034620508</t>
+        </is>
+      </c>
+      <c r="C419" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>16:13:43.887742</t>
+        </is>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F419" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G419" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H419" t="n">
+        <v>7888000</v>
+      </c>
+      <c r="I419" t="n">
+        <v>34000</v>
+      </c>
+      <c r="J419" s="5" t="n">
+        <v>44136.67401181143</v>
+      </c>
+      <c r="K419" s="5" t="n">
+        <v>44136.67620240409</v>
+      </c>
+      <c r="L419" t="inlineStr">
+        <is>
+          <t>0:03:09.267206</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>2020-11-01 161345078556</t>
+        </is>
+      </c>
+      <c r="C420" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>16:16:54.437402</t>
+        </is>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F420" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G420" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H420" t="n">
+        <v>7888000</v>
+      </c>
+      <c r="I420" t="n">
+        <v>34000</v>
+      </c>
+      <c r="J420" s="5" t="n">
+        <v>44136.67621618699</v>
+      </c>
+      <c r="K420" s="5" t="n">
+        <v>44136.67840783998</v>
+      </c>
+      <c r="L420" t="inlineStr">
+        <is>
+          <t>0:03:09.358818</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>2020-11-01 161657912570</t>
+        </is>
+      </c>
+      <c r="C421" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>16:20:18.505992</t>
+        </is>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F421" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G421" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H421" t="n">
+        <v>8352000</v>
+      </c>
+      <c r="I421" t="n">
+        <v>36000</v>
+      </c>
+      <c r="J421" s="5" t="n">
+        <v>44136.67844806215</v>
+      </c>
+      <c r="K421" s="5" t="n">
+        <v>44136.68076974494</v>
+      </c>
+      <c r="L421" t="inlineStr">
+        <is>
+          <t>0:03:20.593394</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>2020-11-01 162019691873</t>
+        </is>
+      </c>
+      <c r="C422" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>16:23:40.153409</t>
+        </is>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F422" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G422" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H422" t="n">
+        <v>8352000</v>
+      </c>
+      <c r="I422" t="n">
+        <v>36000</v>
+      </c>
+      <c r="J422" s="5" t="n">
+        <v>44136.68078347075</v>
+      </c>
+      <c r="K422" s="5" t="n">
+        <v>44136.6831036271</v>
+      </c>
+      <c r="L422" t="inlineStr">
+        <is>
+          <t>0:03:20.461509</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>2020-11-01 162343650531</t>
+        </is>
+      </c>
+      <c r="C423" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>16:27:15.380381</t>
+        </is>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F423" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G423" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H423" t="n">
+        <v>8816000</v>
+      </c>
+      <c r="I423" t="n">
+        <v>38000</v>
+      </c>
+      <c r="J423" s="5" t="n">
+        <v>44136.68314410336</v>
+      </c>
+      <c r="K423" s="5" t="n">
+        <v>44136.68559468001</v>
+      </c>
+      <c r="L423" t="inlineStr">
+        <is>
+          <t>0:03:31.729822</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>2020-11-01 162716572126</t>
+        </is>
+      </c>
+      <c r="C424" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>16:30:47.973726</t>
+        </is>
+      </c>
+      <c r="E424" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F424" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G424" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H424" t="n">
+        <v>8816000</v>
+      </c>
+      <c r="I424" t="n">
+        <v>38000</v>
+      </c>
+      <c r="J424" s="5" t="n">
+        <v>44136.68560847368</v>
+      </c>
+      <c r="K424" s="5" t="n">
+        <v>44136.68805525114</v>
+      </c>
+      <c r="L424" t="inlineStr">
+        <is>
+          <t>0:03:31.401573</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>2020-11-01 163051482553</t>
+        </is>
+      </c>
+      <c r="C425" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>16:34:34.234577</t>
+        </is>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F425" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G425" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H425" t="n">
+        <v>9280000</v>
+      </c>
+      <c r="I425" t="n">
+        <v>40000</v>
+      </c>
+      <c r="J425" s="5" t="n">
+        <v>44136.68809586288</v>
+      </c>
+      <c r="K425" s="5" t="n">
+        <v>44136.690674011</v>
+      </c>
+      <c r="L425" t="inlineStr">
+        <is>
+          <t>0:03:42.751997</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>2020-11-01 163435428074</t>
+        </is>
+      </c>
+      <c r="C426" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>16:38:18.460914</t>
+        </is>
+      </c>
+      <c r="E426" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F426" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G426" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H426" t="n">
+        <v>9280000</v>
+      </c>
+      <c r="I426" t="n">
+        <v>40000</v>
+      </c>
+      <c r="J426" s="5" t="n">
+        <v>44136.69068782493</v>
+      </c>
+      <c r="K426" s="5" t="n">
+        <v>44136.69326922321</v>
+      </c>
+      <c r="L426" t="inlineStr">
+        <is>
+          <t>0:03:43.032811</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>2020-11-01 163822004105</t>
+        </is>
+      </c>
+      <c r="C427" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>16:42:17.111651</t>
+        </is>
+      </c>
+      <c r="E427" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F427" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G427" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H427" t="n">
+        <v>9744000</v>
+      </c>
+      <c r="I427" t="n">
+        <v>42000</v>
+      </c>
+      <c r="J427" s="5" t="n">
+        <v>44136.69331023269</v>
+      </c>
+      <c r="K427" s="5" t="n">
+        <v>44136.69603138457</v>
+      </c>
+      <c r="L427" t="inlineStr">
+        <is>
+          <t>0:03:55.107522</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>2020-11-01 164218318543</t>
+        </is>
+      </c>
+      <c r="C428" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>16:46:12.095707</t>
+        </is>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F428" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G428" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H428" t="n">
+        <v>9744000</v>
+      </c>
+      <c r="I428" t="n">
+        <v>42000</v>
+      </c>
+      <c r="J428" s="5" t="n">
+        <v>44136.69604535351</v>
+      </c>
+      <c r="K428" s="5" t="n">
+        <v>44136.6987511074</v>
+      </c>
+      <c r="L428" t="inlineStr">
+        <is>
+          <t>0:03:53.777136</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>2020-11-01 164615646761</t>
+        </is>
+      </c>
+      <c r="C429" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>16:50:20.792303</t>
+        </is>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F429" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G429" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H429" t="n">
+        <v>10208000</v>
+      </c>
+      <c r="I429" t="n">
+        <v>44000</v>
+      </c>
+      <c r="J429" s="5" t="n">
+        <v>44136.69879220788</v>
+      </c>
+      <c r="K429" s="5" t="n">
+        <v>44136.70162954024</v>
+      </c>
+      <c r="L429" t="inlineStr">
+        <is>
+          <t>0:04:05.145516</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>2020-11-01 165021994499</t>
+        </is>
+      </c>
+      <c r="C430" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>16:54:27.126486</t>
+        </is>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F430" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G430" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H430" t="n">
+        <v>10208000</v>
+      </c>
+      <c r="I430" t="n">
+        <v>44000</v>
+      </c>
+      <c r="J430" s="5" t="n">
+        <v>44136.70164345485</v>
+      </c>
+      <c r="K430" s="5" t="n">
+        <v>44136.70448063031</v>
+      </c>
+      <c r="L430" t="inlineStr">
+        <is>
+          <t>0:04:05.131960</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>2020-11-01 165430668233</t>
+        </is>
+      </c>
+      <c r="C431" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>16:58:46.714363</t>
+        </is>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F431" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G431" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H431" t="n">
+        <v>10672000</v>
+      </c>
+      <c r="I431" t="n">
+        <v>46000</v>
+      </c>
+      <c r="J431" s="5" t="n">
+        <v>44136.70452162307</v>
+      </c>
+      <c r="K431" s="5" t="n">
+        <v>44136.70748511962</v>
+      </c>
+      <c r="L431" t="inlineStr">
+        <is>
+          <t>0:04:16.046102</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>2020-11-01 165847955780</t>
+        </is>
+      </c>
+      <c r="C432" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>17:03:03.577127</t>
+        </is>
+      </c>
+      <c r="E432" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F432" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G432" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H432" t="n">
+        <v>10672000</v>
+      </c>
+      <c r="I432" t="n">
+        <v>46000</v>
+      </c>
+      <c r="J432" s="5" t="n">
+        <v>44136.70749948819</v>
+      </c>
+      <c r="K432" s="5" t="n">
+        <v>44136.71045806828</v>
+      </c>
+      <c r="L432" t="inlineStr">
+        <is>
+          <t>0:04:15.621319</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>2020-11-01 170307141062</t>
+        </is>
+      </c>
+      <c r="C433" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>17:07:34.676233</t>
+        </is>
+      </c>
+      <c r="E433" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F433" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G433" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H433" t="n">
+        <v>11136000</v>
+      </c>
+      <c r="I433" t="n">
+        <v>48000</v>
+      </c>
+      <c r="J433" s="5" t="n">
+        <v>44136.71049931784</v>
+      </c>
+      <c r="K433" s="5" t="n">
+        <v>44136.71359578944</v>
+      </c>
+      <c r="L433" t="inlineStr">
+        <is>
+          <t>0:04:27.535145</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>2020-11-01 170735902297</t>
+        </is>
+      </c>
+      <c r="C434" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>17:12:03.017886</t>
+        </is>
+      </c>
+      <c r="E434" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F434" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G434" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H434" t="n">
+        <v>11136000</v>
+      </c>
+      <c r="I434" t="n">
+        <v>48000</v>
+      </c>
+      <c r="J434" s="5" t="n">
+        <v>44136.71360998029</v>
+      </c>
+      <c r="K434" s="5" t="n">
+        <v>44136.71670159562</v>
+      </c>
+      <c r="L434" t="inlineStr">
+        <is>
+          <t>0:04:27.115565</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>2020-11-01 171206560387</t>
+        </is>
+      </c>
+      <c r="C435" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>17:16:45.052235</t>
+        </is>
+      </c>
+      <c r="E435" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F435" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G435" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H435" t="n">
+        <v>11600000</v>
+      </c>
+      <c r="I435" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J435" s="5" t="n">
+        <v>44136.71674259707</v>
+      </c>
+      <c r="K435" s="5" t="n">
+        <v>44136.71996588202</v>
+      </c>
+      <c r="L435" t="inlineStr">
+        <is>
+          <t>0:04:38.491819</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>2020-11-01 171646279081</t>
+        </is>
+      </c>
+      <c r="C436" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>17:21:24.966688</t>
+        </is>
+      </c>
+      <c r="E436" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F436" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G436" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H436" t="n">
+        <v>11600000</v>
+      </c>
+      <c r="I436" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J436" s="5" t="n">
+        <v>44136.71998008196</v>
+      </c>
+      <c r="K436" s="5" t="n">
+        <v>44136.72320563254</v>
+      </c>
+      <c r="L436" t="inlineStr">
+        <is>
+          <t>0:04:38.687570</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>2020-11-01 172128545807</t>
+        </is>
+      </c>
+      <c r="C437" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>17:26:18.734990</t>
+        </is>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G437" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H437" t="n">
+        <v>12064000</v>
+      </c>
+      <c r="I437" t="n">
+        <v>52000</v>
+      </c>
+      <c r="J437" s="5" t="n">
+        <v>44136.72324705795</v>
+      </c>
+      <c r="K437" s="5" t="n">
+        <v>44136.72660572868</v>
+      </c>
+      <c r="L437" t="inlineStr">
+        <is>
+          <t>0:04:50.189151</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>2020-11-01 172619975856</t>
+        </is>
+      </c>
+      <c r="C438" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>17:31:09.888613</t>
+        </is>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H438" t="n">
+        <v>12064000</v>
+      </c>
+      <c r="I438" t="n">
+        <v>52000</v>
+      </c>
+      <c r="J438" s="5" t="n">
+        <v>44136.72662009093</v>
+      </c>
+      <c r="K438" s="5" t="n">
+        <v>44136.7299755623</v>
+      </c>
+      <c r="L438" t="inlineStr">
+        <is>
+          <t>0:04:49.912727</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>2020-11-01 173113480679</t>
+        </is>
+      </c>
+      <c r="C439" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>17:36:14.502645</t>
+        </is>
+      </c>
+      <c r="E439" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F439" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G439" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H439" t="n">
+        <v>12528000</v>
+      </c>
+      <c r="I439" t="n">
+        <v>54000</v>
+      </c>
+      <c r="J439" s="5" t="n">
+        <v>44136.73001713749</v>
+      </c>
+      <c r="K439" s="5" t="n">
+        <v>44136.73350118753</v>
+      </c>
+      <c r="L439" t="inlineStr">
+        <is>
+          <t>0:05:01.021924</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>2020-11-01 173615741106</t>
+        </is>
+      </c>
+      <c r="C440" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>17:41:16.520055</t>
+        </is>
+      </c>
+      <c r="E440" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F440" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G440" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H440" t="n">
+        <v>12528000</v>
+      </c>
+      <c r="I440" t="n">
+        <v>54000</v>
+      </c>
+      <c r="J440" s="5" t="n">
+        <v>44136.73351552206</v>
+      </c>
+      <c r="K440" s="5" t="n">
+        <v>44136.73699675961</v>
+      </c>
+      <c r="L440" t="inlineStr">
+        <is>
+          <t>0:05:00.778923</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>2020-11-01 174120109535</t>
+        </is>
+      </c>
+      <c r="C441" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>17:46:32.342606</t>
+        </is>
+      </c>
+      <c r="E441" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F441" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G441" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H441" t="n">
+        <v>12992000</v>
+      </c>
+      <c r="I441" t="n">
+        <v>56000</v>
+      </c>
+      <c r="J441" s="5" t="n">
+        <v>44136.73703830479</v>
+      </c>
+      <c r="K441" s="5" t="n">
+        <v>44136.74065211321</v>
+      </c>
+      <c r="L441" t="inlineStr">
+        <is>
+          <t>0:05:12.233047</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>2020-11-01 174633571900</t>
+        </is>
+      </c>
+      <c r="C442" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>17:51:45.065716</t>
+        </is>
+      </c>
+      <c r="E442" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F442" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G442" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H442" t="n">
+        <v>12992000</v>
+      </c>
+      <c r="I442" t="n">
+        <v>56000</v>
+      </c>
+      <c r="J442" s="5" t="n">
+        <v>44136.74066634144</v>
+      </c>
+      <c r="K442" s="5" t="n">
+        <v>44136.74427159361</v>
+      </c>
+      <c r="L442" t="inlineStr">
+        <is>
+          <t>0:05:11.493788</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>2020-11-01 175148704321</t>
+        </is>
+      </c>
+      <c r="C443" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>17:57:12.090836</t>
+        </is>
+      </c>
+      <c r="E443" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F443" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G443" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H443" t="n">
+        <v>13456000</v>
+      </c>
+      <c r="I443" t="n">
+        <v>58000</v>
+      </c>
+      <c r="J443" s="5" t="n">
+        <v>44136.74431370742</v>
+      </c>
+      <c r="K443" s="5" t="n">
+        <v>44136.74805660648</v>
+      </c>
+      <c r="L443" t="inlineStr">
+        <is>
+          <t>0:05:23.386479</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>2020-11-01 175713334153</t>
+        </is>
+      </c>
+      <c r="C444" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>18:02:36.161855</t>
+        </is>
+      </c>
+      <c r="E444" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F444" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G444" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H444" t="n">
+        <v>13456000</v>
+      </c>
+      <c r="I444" t="n">
+        <v>58000</v>
+      </c>
+      <c r="J444" s="5" t="n">
+        <v>44136.74807099714</v>
+      </c>
+      <c r="K444" s="5" t="n">
+        <v>44136.7518074286</v>
+      </c>
+      <c r="L444" t="inlineStr">
+        <is>
+          <t>0:05:22.827678</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>2020-11-01 180239780069</t>
+        </is>
+      </c>
+      <c r="C445" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>18:08:14.477013</t>
+        </is>
+      </c>
+      <c r="E445" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F445" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G445" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H445" t="n">
+        <v>13920000</v>
+      </c>
+      <c r="I445" t="n">
+        <v>60000</v>
+      </c>
+      <c r="J445" s="5" t="n">
+        <v>44136.75184930634</v>
+      </c>
+      <c r="K445" s="5" t="n">
+        <v>44136.75572311327</v>
+      </c>
+      <c r="L445" t="inlineStr">
+        <is>
+          <t>0:05:34.696918</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>2020-11-01 180815716077</t>
+        </is>
+      </c>
+      <c r="C446" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>18:13:50.531201</t>
+        </is>
+      </c>
+      <c r="E446" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F446" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G446" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H446" t="n">
+        <v>13920000</v>
+      </c>
+      <c r="I446" t="n">
+        <v>60000</v>
+      </c>
+      <c r="J446" s="5" t="n">
+        <v>44136.75573745459</v>
+      </c>
+      <c r="K446" s="5" t="n">
+        <v>44136.75961262933</v>
+      </c>
+      <c r="L446" t="inlineStr">
+        <is>
+          <t>0:05:34.815097</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>2020-11-01 181354165946</t>
+        </is>
+      </c>
+      <c r="C447" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>18:19:39.784291</t>
+        </is>
+      </c>
+      <c r="E447" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F447" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G447" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H447" t="n">
+        <v>14384000</v>
+      </c>
+      <c r="I447" t="n">
+        <v>62000</v>
+      </c>
+      <c r="J447" s="5" t="n">
+        <v>44136.75965469845</v>
+      </c>
+      <c r="K447" s="5" t="n">
+        <v>44136.7636549105</v>
+      </c>
+      <c r="L447" t="inlineStr">
+        <is>
+          <t>0:05:45.618321</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>2020-11-01 181941033823</t>
+        </is>
+      </c>
+      <c r="C448" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>18:25:26.390006</t>
+        </is>
+      </c>
+      <c r="E448" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F448" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G448" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H448" t="n">
+        <v>14384000</v>
+      </c>
+      <c r="I448" t="n">
+        <v>62000</v>
+      </c>
+      <c r="J448" s="5" t="n">
+        <v>44136.76366937295</v>
+      </c>
+      <c r="K448" s="5" t="n">
+        <v>44136.7676665507</v>
+      </c>
+      <c r="L448" t="inlineStr">
+        <is>
+          <t>0:05:45.356157</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>2020-11-01 182530044497</t>
+        </is>
+      </c>
+      <c r="C449" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>18:31:26.787072</t>
+        </is>
+      </c>
+      <c r="E449" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F449" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G449" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H449" t="n">
+        <v>14848000</v>
+      </c>
+      <c r="I449" t="n">
+        <v>64000</v>
+      </c>
+      <c r="J449" s="5" t="n">
+        <v>44136.76770884835</v>
+      </c>
+      <c r="K449" s="5" t="n">
+        <v>44136.771837813</v>
+      </c>
+      <c r="L449" t="inlineStr">
+        <is>
+          <t>0:05:56.742546</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>2020-11-01 183128024309</t>
+        </is>
+      </c>
+      <c r="C450" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>18:37:24.650125</t>
+        </is>
+      </c>
+      <c r="E450" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F450" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G450" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H450" t="n">
+        <v>14848000</v>
+      </c>
+      <c r="I450" t="n">
+        <v>64000</v>
+      </c>
+      <c r="J450" s="5" t="n">
+        <v>44136.77185213322</v>
+      </c>
+      <c r="K450" s="5" t="n">
+        <v>44136.77597974648</v>
+      </c>
+      <c r="L450" t="inlineStr">
+        <is>
+          <t>0:05:56.625787</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>2020-11-01 183728324868</t>
+        </is>
+      </c>
+      <c r="C451" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>18:43:38.156354</t>
+        </is>
+      </c>
+      <c r="E451" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F451" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G451" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H451" t="n">
+        <v>15312000</v>
+      </c>
+      <c r="I451" t="n">
+        <v>66000</v>
+      </c>
+      <c r="J451" s="5" t="n">
+        <v>44136.77602227857</v>
+      </c>
+      <c r="K451" s="5" t="n">
+        <v>44136.78030273528</v>
+      </c>
+      <c r="L451" t="inlineStr">
+        <is>
+          <t>0:06:09.831460</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>2020-11-01 184339410575</t>
+        </is>
+      </c>
+      <c r="C452" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>18:49:46.940695</t>
+        </is>
+      </c>
+      <c r="E452" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F452" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G452" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H452" t="n">
+        <v>15312000</v>
+      </c>
+      <c r="I452" t="n">
+        <v>66000</v>
+      </c>
+      <c r="J452" s="5" t="n">
+        <v>44136.78031725203</v>
+      </c>
+      <c r="K452" s="5" t="n">
+        <v>44136.78457107256</v>
+      </c>
+      <c r="L452" t="inlineStr">
+        <is>
+          <t>0:06:07.530094</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>2020-11-01 184950609484</t>
+        </is>
+      </c>
+      <c r="C453" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>18:56:10.087342</t>
+        </is>
+      </c>
+      <c r="E453" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F453" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G453" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H453" t="n">
+        <v>15776000</v>
+      </c>
+      <c r="I453" t="n">
+        <v>68000</v>
+      </c>
+      <c r="J453" s="5" t="n">
+        <v>44136.7846135357</v>
+      </c>
+      <c r="K453" s="5" t="n">
+        <v>44136.78900564023</v>
+      </c>
+      <c r="L453" t="inlineStr">
+        <is>
+          <t>0:06:19.477832</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>2020-11-01 185611325519</t>
+        </is>
+      </c>
+      <c r="C454" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>19:02:30.282498</t>
+        </is>
+      </c>
+      <c r="E454" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F454" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G454" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H454" t="n">
+        <v>15776000</v>
+      </c>
+      <c r="I454" t="n">
+        <v>68000</v>
+      </c>
+      <c r="J454" s="5" t="n">
+        <v>44136.78901997129</v>
+      </c>
+      <c r="K454" s="5" t="n">
+        <v>44136.79340604691</v>
+      </c>
+      <c r="L454" t="inlineStr">
+        <is>
+          <t>0:06:18.956934</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>2020-11-01 190233997967</t>
+        </is>
+      </c>
+      <c r="C455" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D455" t="inlineStr">
+        <is>
+          <t>19:09:04.365251</t>
+        </is>
+      </c>
+      <c r="E455" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F455" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G455" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H455" t="n">
+        <v>16240000</v>
+      </c>
+      <c r="I455" t="n">
+        <v>70000</v>
+      </c>
+      <c r="J455" s="5" t="n">
+        <v>44136.79344905054</v>
+      </c>
+      <c r="K455" s="5" t="n">
+        <v>44136.79796719009</v>
+      </c>
+      <c r="L455" t="inlineStr">
+        <is>
+          <t>0:06:30.367258</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>2020-11-01 190905603980</t>
+        </is>
+      </c>
+      <c r="C456" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>19:15:35.262576</t>
+        </is>
+      </c>
+      <c r="E456" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F456" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G456" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H456" t="n">
+        <v>16240000</v>
+      </c>
+      <c r="I456" t="n">
+        <v>70000</v>
+      </c>
+      <c r="J456" s="5" t="n">
+        <v>44136.79798152755</v>
+      </c>
+      <c r="K456" s="5" t="n">
+        <v>44136.80249146469</v>
+      </c>
+      <c r="L456" t="inlineStr">
+        <is>
+          <t>0:06:29.658569</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>2020-11-01 191539031578</t>
+        </is>
+      </c>
+      <c r="C457" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>19:22:20.331960</t>
+        </is>
+      </c>
+      <c r="E457" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F457" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G457" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H457" t="n">
+        <v>16704000</v>
+      </c>
+      <c r="I457" t="n">
+        <v>72000</v>
+      </c>
+      <c r="J457" s="5" t="n">
+        <v>44136.80253508771</v>
+      </c>
+      <c r="K457" s="5" t="n">
+        <v>44136.80717976772</v>
+      </c>
+      <c r="L457" t="inlineStr">
+        <is>
+          <t>0:06:41.300353</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>2020-11-01 192221570691</t>
+        </is>
+      </c>
+      <c r="C458" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>19:29:02.893354</t>
+        </is>
+      </c>
+      <c r="E458" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F458" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G458" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H458" t="n">
+        <v>16704000</v>
+      </c>
+      <c r="I458" t="n">
+        <v>72000</v>
+      </c>
+      <c r="J458" s="5" t="n">
+        <v>44136.80719410522</v>
+      </c>
+      <c r="K458" s="5" t="n">
+        <v>44136.81183904313</v>
+      </c>
+      <c r="L458" t="inlineStr">
+        <is>
+          <t>0:06:41.322636</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>2020-11-01 192906631358</t>
+        </is>
+      </c>
+      <c r="C459" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D459" t="inlineStr">
+        <is>
+          <t>19:35:59.048563</t>
+        </is>
+      </c>
+      <c r="E459" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F459" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G459" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H459" t="n">
+        <v>17168000</v>
+      </c>
+      <c r="I459" t="n">
+        <v>74000</v>
+      </c>
+      <c r="J459" s="5" t="n">
+        <v>44136.81188230738</v>
+      </c>
+      <c r="K459" s="5" t="n">
+        <v>44136.81665565435</v>
+      </c>
+      <c r="L459" t="inlineStr">
+        <is>
+          <t>0:06:52.417178</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>2020-11-01 193600288116</t>
+        </is>
+      </c>
+      <c r="C460" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D460" t="inlineStr">
+        <is>
+          <t>19:42:52.593936</t>
+        </is>
+      </c>
+      <c r="E460" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F460" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G460" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H460" t="n">
+        <v>17168000</v>
+      </c>
+      <c r="I460" t="n">
+        <v>74000</v>
+      </c>
+      <c r="J460" s="5" t="n">
+        <v>44136.81667000135</v>
+      </c>
+      <c r="K460" s="5" t="n">
+        <v>44136.82144205913</v>
+      </c>
+      <c r="L460" t="inlineStr">
+        <is>
+          <t>0:06:52.305793</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>2020-11-01 194256330619</t>
+        </is>
+      </c>
+      <c r="C461" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>19:50:00.527389</t>
+        </is>
+      </c>
+      <c r="E461" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F461" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G461" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H461" t="n">
+        <v>17632000</v>
+      </c>
+      <c r="I461" t="n">
+        <v>76000</v>
+      </c>
+      <c r="J461" s="5" t="n">
+        <v>44136.82148530809</v>
+      </c>
+      <c r="K461" s="5" t="n">
+        <v>44136.82639499262</v>
+      </c>
+      <c r="L461" t="inlineStr">
+        <is>
+          <t>0:07:04.196743</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>2020-11-01 195001770228</t>
+        </is>
+      </c>
+      <c r="C462" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>19:57:05.172246</t>
+        </is>
+      </c>
+      <c r="E462" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F462" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G462" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H462" t="n">
+        <v>17632000</v>
+      </c>
+      <c r="I462" t="n">
+        <v>76000</v>
+      </c>
+      <c r="J462" s="5" t="n">
+        <v>44136.82640937764</v>
+      </c>
+      <c r="K462" s="5" t="n">
+        <v>44136.83130986364</v>
+      </c>
+      <c r="L462" t="inlineStr">
+        <is>
+          <t>0:07:03.401990</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>2020-11-01 195708938462</t>
+        </is>
+      </c>
+      <c r="C463" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>20:04:24.257332</t>
+        </is>
+      </c>
+      <c r="E463" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F463" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G463" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H463" t="n">
+        <v>18096000</v>
+      </c>
+      <c r="I463" t="n">
+        <v>78000</v>
+      </c>
+      <c r="J463" s="5" t="n">
+        <v>44136.83135345442</v>
+      </c>
+      <c r="K463" s="5" t="n">
+        <v>44136.83639186696</v>
+      </c>
+      <c r="L463" t="inlineStr">
+        <is>
+          <t>0:07:15.318843</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>2020-11-01 200425507372</t>
+        </is>
+      </c>
+      <c r="C464" s="4" t="n">
+        <v>44136</v>
+      </c>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>20:11:40.075552</t>
+        </is>
+      </c>
+      <c r="E464" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F464" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G464" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H464" t="n">
+        <v>18096000</v>
+      </c>
+      <c r="I464" t="n">
+        <v>78000</v>
+      </c>
+      <c r="J464" s="5" t="n">
+        <v>44136.83640633532</v>
+      </c>
+      <c r="K464" s="5" t="n">
+        <v>44136.84143605929</v>
+      </c>
+      <c r="L464" t="inlineStr">
+        <is>
+          <t>0:07:14.568151</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
added(experiment_nosql) 50.000 increment tests.
</commit_message>
<xml_diff>
--- a/experiment_nosql.xlsx
+++ b/experiment_nosql.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L464"/>
+  <dimension ref="A1:L504"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
@@ -23663,11 +23663,2011 @@
         <v>44136.83640633532</v>
       </c>
       <c r="K464" s="5" t="n">
-        <v>44136.84143605929</v>
+        <v>44136.84143605928</v>
       </c>
       <c r="L464" t="inlineStr">
         <is>
           <t>0:07:14.568151</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>2020-11-21 160038476312</t>
+        </is>
+      </c>
+      <c r="C465" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D465" t="inlineStr">
+        <is>
+          <t>16:05:14.041348</t>
+        </is>
+      </c>
+      <c r="E465" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F465" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G465" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H465" t="n">
+        <v>11600000</v>
+      </c>
+      <c r="I465" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J465" s="5" t="n">
+        <v>44156.66711199435</v>
+      </c>
+      <c r="K465" s="5" t="n">
+        <v>44156.67030140416</v>
+      </c>
+      <c r="L465" t="inlineStr">
+        <is>
+          <t>0:04:35.565007</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>2020-11-21 160515533670</t>
+        </is>
+      </c>
+      <c r="C466" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D466" t="inlineStr">
+        <is>
+          <t>16:09:52.859765</t>
+        </is>
+      </c>
+      <c r="E466" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F466" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G466" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H466" t="n">
+        <v>11600000</v>
+      </c>
+      <c r="I466" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J466" s="5" t="n">
+        <v>44156.67031867673</v>
+      </c>
+      <c r="K466" s="5" t="n">
+        <v>44156.67352846915</v>
+      </c>
+      <c r="L466" t="inlineStr">
+        <is>
+          <t>0:04:37.326065</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>2020-11-21 160956522671</t>
+        </is>
+      </c>
+      <c r="C467" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D467" t="inlineStr">
+        <is>
+          <t>16:19:06.399550</t>
+        </is>
+      </c>
+      <c r="E467" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F467" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G467" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H467" t="n">
+        <v>23200000</v>
+      </c>
+      <c r="I467" t="n">
+        <v>100000</v>
+      </c>
+      <c r="J467" s="5" t="n">
+        <v>44156.67357086424</v>
+      </c>
+      <c r="K467" s="5" t="n">
+        <v>44156.67993517967</v>
+      </c>
+      <c r="L467" t="inlineStr">
+        <is>
+          <t>0:09:09.876853</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>2020-11-21 161907627186</t>
+        </is>
+      </c>
+      <c r="C468" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D468" t="inlineStr">
+        <is>
+          <t>16:28:15.010856</t>
+        </is>
+      </c>
+      <c r="E468" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F468" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G468" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H468" t="n">
+        <v>23200000</v>
+      </c>
+      <c r="I468" t="n">
+        <v>100000</v>
+      </c>
+      <c r="J468" s="5" t="n">
+        <v>44156.67994938873</v>
+      </c>
+      <c r="K468" s="5" t="n">
+        <v>44156.68628484749</v>
+      </c>
+      <c r="L468" t="inlineStr">
+        <is>
+          <t>0:09:07.383637</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>2020-11-21 162818917670</t>
+        </is>
+      </c>
+      <c r="C469" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D469" t="inlineStr">
+        <is>
+          <t>16:42:01.366100</t>
+        </is>
+      </c>
+      <c r="E469" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F469" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G469" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H469" t="n">
+        <v>34800000</v>
+      </c>
+      <c r="I469" t="n">
+        <v>150000</v>
+      </c>
+      <c r="J469" s="5" t="n">
+        <v>44156.68633006563</v>
+      </c>
+      <c r="K469" s="5" t="n">
+        <v>44156.69584914439</v>
+      </c>
+      <c r="L469" t="inlineStr">
+        <is>
+          <t>0:13:42.448405</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>2020-11-21 164202606377</t>
+        </is>
+      </c>
+      <c r="C470" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D470" t="inlineStr">
+        <is>
+          <t>16:55:43.640639</t>
+        </is>
+      </c>
+      <c r="E470" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F470" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G470" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H470" t="n">
+        <v>34800000</v>
+      </c>
+      <c r="I470" t="n">
+        <v>150000</v>
+      </c>
+      <c r="J470" s="5" t="n">
+        <v>44156.69586349974</v>
+      </c>
+      <c r="K470" s="5" t="n">
+        <v>44156.70536621082</v>
+      </c>
+      <c r="L470" t="inlineStr">
+        <is>
+          <t>0:13:41.034238</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>2020-11-21 165547909264</t>
+        </is>
+      </c>
+      <c r="C471" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D471" t="inlineStr">
+        <is>
+          <t>17:14:11.498814</t>
+        </is>
+      </c>
+      <c r="E471" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F471" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G471" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H471" t="n">
+        <v>46400000</v>
+      </c>
+      <c r="I471" t="n">
+        <v>200000</v>
+      </c>
+      <c r="J471" s="5" t="n">
+        <v>44156.70541561648</v>
+      </c>
+      <c r="K471" s="5" t="n">
+        <v>44156.71818864338</v>
+      </c>
+      <c r="L471" t="inlineStr">
+        <is>
+          <t>0:18:23.589524</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>2020-11-21 171412742939</t>
+        </is>
+      </c>
+      <c r="C472" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D472" t="inlineStr">
+        <is>
+          <t>17:32:32.165390</t>
+        </is>
+      </c>
+      <c r="E472" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F472" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G472" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H472" t="n">
+        <v>46400000</v>
+      </c>
+      <c r="I472" t="n">
+        <v>200000</v>
+      </c>
+      <c r="J472" s="5" t="n">
+        <v>44156.71820304327</v>
+      </c>
+      <c r="K472" s="5" t="n">
+        <v>44156.73092783986</v>
+      </c>
+      <c r="L472" t="inlineStr">
+        <is>
+          <t>0:18:19.422425</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>2020-11-21 173236815010</t>
+        </is>
+      </c>
+      <c r="C473" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D473" t="inlineStr">
+        <is>
+          <t>17:55:36.855893</t>
+        </is>
+      </c>
+      <c r="E473" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F473" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G473" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H473" t="n">
+        <v>58000000</v>
+      </c>
+      <c r="I473" t="n">
+        <v>250000</v>
+      </c>
+      <c r="J473" s="5" t="n">
+        <v>44156.73098165521</v>
+      </c>
+      <c r="K473" s="5" t="n">
+        <v>44156.74695435035</v>
+      </c>
+      <c r="L473" t="inlineStr">
+        <is>
+          <t>0:23:00.040860</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>2020-11-21 175538104192</t>
+        </is>
+      </c>
+      <c r="C474" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D474" t="inlineStr">
+        <is>
+          <t>18:18:33.642849</t>
+        </is>
+      </c>
+      <c r="E474" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F474" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G474" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H474" t="n">
+        <v>58000000</v>
+      </c>
+      <c r="I474" t="n">
+        <v>250000</v>
+      </c>
+      <c r="J474" s="5" t="n">
+        <v>44156.74696879852</v>
+      </c>
+      <c r="K474" s="5" t="n">
+        <v>44156.76288938451</v>
+      </c>
+      <c r="L474" t="inlineStr">
+        <is>
+          <t>0:22:55.538630</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>2020-11-21 181838653318</t>
+        </is>
+      </c>
+      <c r="C475" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D475" t="inlineStr">
+        <is>
+          <t>18:46:14.651852</t>
+        </is>
+      </c>
+      <c r="E475" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F475" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G475" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H475" t="n">
+        <v>69600000</v>
+      </c>
+      <c r="I475" t="n">
+        <v>300000</v>
+      </c>
+      <c r="J475" s="5" t="n">
+        <v>44156.76294737638</v>
+      </c>
+      <c r="K475" s="5" t="n">
+        <v>44156.7821140258</v>
+      </c>
+      <c r="L475" t="inlineStr">
+        <is>
+          <t>0:27:35.998511</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>2020-11-21 184615935289</t>
+        </is>
+      </c>
+      <c r="C476" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D476" t="inlineStr">
+        <is>
+          <t>19:13:47.862359</t>
+        </is>
+      </c>
+      <c r="E476" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F476" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G476" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H476" t="n">
+        <v>69600000</v>
+      </c>
+      <c r="I476" t="n">
+        <v>300000</v>
+      </c>
+      <c r="J476" s="5" t="n">
+        <v>44156.78212888066</v>
+      </c>
+      <c r="K476" s="5" t="n">
+        <v>44156.80124840662</v>
+      </c>
+      <c r="L476" t="inlineStr">
+        <is>
+          <t>0:27:31.927043</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>2020-11-21 191353156911</t>
+        </is>
+      </c>
+      <c r="C477" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D477" t="inlineStr">
+        <is>
+          <t>19:46:15.292759</t>
+        </is>
+      </c>
+      <c r="E477" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F477" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G477" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H477" t="n">
+        <v>81200000</v>
+      </c>
+      <c r="I477" t="n">
+        <v>350000</v>
+      </c>
+      <c r="J477" s="5" t="n">
+        <v>44156.80130968647</v>
+      </c>
+      <c r="K477" s="5" t="n">
+        <v>44156.82378811033</v>
+      </c>
+      <c r="L477" t="inlineStr">
+        <is>
+          <t>0:32:22.135821</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>2020-11-21 194616586961</t>
+        </is>
+      </c>
+      <c r="C478" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D478" t="inlineStr">
+        <is>
+          <t>20:18:23.683629</t>
+        </is>
+      </c>
+      <c r="E478" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F478" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G478" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H478" t="n">
+        <v>81200000</v>
+      </c>
+      <c r="I478" t="n">
+        <v>350000</v>
+      </c>
+      <c r="J478" s="5" t="n">
+        <v>44156.82380308983</v>
+      </c>
+      <c r="K478" s="5" t="n">
+        <v>44156.84610744908</v>
+      </c>
+      <c r="L478" t="inlineStr">
+        <is>
+          <t>0:32:07.096639</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>2020-11-21 201829211481</t>
+        </is>
+      </c>
+      <c r="C479" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D479" t="inlineStr">
+        <is>
+          <t>20:55:17.457919</t>
+        </is>
+      </c>
+      <c r="E479" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F479" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G479" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H479" t="n">
+        <v>92800000</v>
+      </c>
+      <c r="I479" t="n">
+        <v>400000</v>
+      </c>
+      <c r="J479" s="5" t="n">
+        <v>44156.84617142918</v>
+      </c>
+      <c r="K479" s="5" t="n">
+        <v>44156.87172983673</v>
+      </c>
+      <c r="L479" t="inlineStr">
+        <is>
+          <t>0:36:48.246413</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>2020-11-21 205518743809</t>
+        </is>
+      </c>
+      <c r="C480" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D480" t="inlineStr">
+        <is>
+          <t>21:32:02.002237</t>
+        </is>
+      </c>
+      <c r="E480" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F480" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G480" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H480" t="n">
+        <v>92800000</v>
+      </c>
+      <c r="I480" t="n">
+        <v>400000</v>
+      </c>
+      <c r="J480" s="5" t="n">
+        <v>44156.87174472001</v>
+      </c>
+      <c r="K480" s="5" t="n">
+        <v>44156.89724539597</v>
+      </c>
+      <c r="L480" t="inlineStr">
+        <is>
+          <t>0:36:43.258403</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>2020-11-21 213207931009</t>
+        </is>
+      </c>
+      <c r="C481" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D481" t="inlineStr">
+        <is>
+          <t>22:13:33.308544</t>
+        </is>
+      </c>
+      <c r="E481" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F481" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G481" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H481" t="n">
+        <v>104400000</v>
+      </c>
+      <c r="I481" t="n">
+        <v>450000</v>
+      </c>
+      <c r="J481" s="5" t="n">
+        <v>44156.89731401631</v>
+      </c>
+      <c r="K481" s="5" t="n">
+        <v>44156.92607995975</v>
+      </c>
+      <c r="L481" t="inlineStr">
+        <is>
+          <t>0:41:25.377513</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>2020-11-21 221334617305</t>
+        </is>
+      </c>
+      <c r="C482" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D482" t="inlineStr">
+        <is>
+          <t>22:54:35.905636</t>
+        </is>
+      </c>
+      <c r="E482" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F482" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G482" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H482" t="n">
+        <v>104400000</v>
+      </c>
+      <c r="I482" t="n">
+        <v>450000</v>
+      </c>
+      <c r="J482" s="5" t="n">
+        <v>44156.92609510769</v>
+      </c>
+      <c r="K482" s="5" t="n">
+        <v>44156.95458224085</v>
+      </c>
+      <c r="L482" t="inlineStr">
+        <is>
+          <t>0:41:01.288304</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>2020-11-21 225442122582</t>
+        </is>
+      </c>
+      <c r="C483" s="4" t="n">
+        <v>44156</v>
+      </c>
+      <c r="D483" t="inlineStr">
+        <is>
+          <t>23:40:27.108155</t>
+        </is>
+      </c>
+      <c r="E483" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F483" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G483" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H483" t="n">
+        <v>116000000</v>
+      </c>
+      <c r="I483" t="n">
+        <v>500000</v>
+      </c>
+      <c r="J483" s="5" t="n">
+        <v>44156.95465419655</v>
+      </c>
+      <c r="K483" s="5" t="n">
+        <v>44156.98642486264</v>
+      </c>
+      <c r="L483" t="inlineStr">
+        <is>
+          <t>0:45:44.985550</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>2020-11-21 234028403241</t>
+        </is>
+      </c>
+      <c r="C484" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D484" t="inlineStr">
+        <is>
+          <t>00:26:01.109898</t>
+        </is>
+      </c>
+      <c r="E484" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F484" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G484" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H484" t="n">
+        <v>116000000</v>
+      </c>
+      <c r="I484" t="n">
+        <v>500000</v>
+      </c>
+      <c r="J484" s="5" t="n">
+        <v>44156.98643985233</v>
+      </c>
+      <c r="K484" s="5" t="n">
+        <v>44157.01806840126</v>
+      </c>
+      <c r="L484" t="inlineStr">
+        <is>
+          <t>0:45:32.706629</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>2020-11-22 002607724428</t>
+        </is>
+      </c>
+      <c r="C485" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D485" t="inlineStr">
+        <is>
+          <t>01:16:26.908870</t>
+        </is>
+      </c>
+      <c r="E485" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F485" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G485" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H485" t="n">
+        <v>127600000</v>
+      </c>
+      <c r="I485" t="n">
+        <v>550000</v>
+      </c>
+      <c r="J485" s="5" t="n">
+        <v>44157.01814495866</v>
+      </c>
+      <c r="K485" s="5" t="n">
+        <v>44157.05308922272</v>
+      </c>
+      <c r="L485" t="inlineStr">
+        <is>
+          <t>0:50:19.184415</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>2020-11-22 011628215515</t>
+        </is>
+      </c>
+      <c r="C486" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>02:06:38.087501</t>
+        </is>
+      </c>
+      <c r="E486" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F486" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G486" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H486" t="n">
+        <v>127600000</v>
+      </c>
+      <c r="I486" t="n">
+        <v>550000</v>
+      </c>
+      <c r="J486" s="5" t="n">
+        <v>44157.05310434624</v>
+      </c>
+      <c r="K486" s="5" t="n">
+        <v>44157.08794082715</v>
+      </c>
+      <c r="L486" t="inlineStr">
+        <is>
+          <t>0:50:09.871951</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>2020-11-22 020644883622</t>
+        </is>
+      </c>
+      <c r="C487" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D487" t="inlineStr">
+        <is>
+          <t>03:01:38.446796</t>
+        </is>
+      </c>
+      <c r="E487" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F487" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G487" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H487" t="n">
+        <v>139200000</v>
+      </c>
+      <c r="I487" t="n">
+        <v>600000</v>
+      </c>
+      <c r="J487" s="5" t="n">
+        <v>44157.08801948636</v>
+      </c>
+      <c r="K487" s="5" t="n">
+        <v>44157.12613943021</v>
+      </c>
+      <c r="L487" t="inlineStr">
+        <is>
+          <t>0:54:53.563148</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>2020-11-22 030139754241</t>
+        </is>
+      </c>
+      <c r="C488" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>03:56:26.212418</t>
+        </is>
+      </c>
+      <c r="E488" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F488" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G488" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H488" t="n">
+        <v>139200000</v>
+      </c>
+      <c r="I488" t="n">
+        <v>600000</v>
+      </c>
+      <c r="J488" s="5" t="n">
+        <v>44157.12615456296</v>
+      </c>
+      <c r="K488" s="5" t="n">
+        <v>44157.16419227303</v>
+      </c>
+      <c r="L488" t="inlineStr">
+        <is>
+          <t>0:54:46.458149</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>2020-11-22 035633488725</t>
+        </is>
+      </c>
+      <c r="C489" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>04:56:03.018949</t>
+        </is>
+      </c>
+      <c r="E489" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F489" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G489" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H489" t="n">
+        <v>150800000</v>
+      </c>
+      <c r="I489" t="n">
+        <v>650000</v>
+      </c>
+      <c r="J489" s="5" t="n">
+        <v>44157.16427648987</v>
+      </c>
+      <c r="K489" s="5" t="n">
+        <v>44157.20559049679</v>
+      </c>
+      <c r="L489" t="inlineStr">
+        <is>
+          <t>0:59:29.530198</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>2020-11-22 045604339388</t>
+        </is>
+      </c>
+      <c r="C490" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>05:55:17.304102</t>
+        </is>
+      </c>
+      <c r="E490" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F490" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G490" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H490" t="n">
+        <v>150800000</v>
+      </c>
+      <c r="I490" t="n">
+        <v>650000</v>
+      </c>
+      <c r="J490" s="5" t="n">
+        <v>44157.20560577996</v>
+      </c>
+      <c r="K490" s="5" t="n">
+        <v>44157.24672805646</v>
+      </c>
+      <c r="L490" t="inlineStr">
+        <is>
+          <t>0:59:12.964690</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>2020-11-22 055524862253</t>
+        </is>
+      </c>
+      <c r="C491" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>06:59:30.004348</t>
+        </is>
+      </c>
+      <c r="E491" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F491" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G491" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H491" t="n">
+        <v>162400000</v>
+      </c>
+      <c r="I491" t="n">
+        <v>700000</v>
+      </c>
+      <c r="J491" s="5" t="n">
+        <v>44157.24681553533</v>
+      </c>
+      <c r="K491" s="5" t="n">
+        <v>44157.29131949447</v>
+      </c>
+      <c r="L491" t="inlineStr">
+        <is>
+          <t>1:04:05.142069</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>2020-11-22 065931651003</t>
+        </is>
+      </c>
+      <c r="C492" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>08:03:56.720848</t>
+        </is>
+      </c>
+      <c r="E492" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F492" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G492" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H492" t="n">
+        <v>162400000</v>
+      </c>
+      <c r="I492" t="n">
+        <v>700000</v>
+      </c>
+      <c r="J492" s="5" t="n">
+        <v>44157.29133855327</v>
+      </c>
+      <c r="K492" s="5" t="n">
+        <v>44157.33607315762</v>
+      </c>
+      <c r="L492" t="inlineStr">
+        <is>
+          <t>1:04:25.069816</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>2020-11-22 080404720319</t>
+        </is>
+      </c>
+      <c r="C493" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>09:12:00.599347</t>
+        </is>
+      </c>
+      <c r="E493" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F493" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G493" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H493" t="n">
+        <v>174000000</v>
+      </c>
+      <c r="I493" t="n">
+        <v>750000</v>
+      </c>
+      <c r="J493" s="5" t="n">
+        <v>44157.33616574443</v>
+      </c>
+      <c r="K493" s="5" t="n">
+        <v>44157.38334026993</v>
+      </c>
+      <c r="L493" t="inlineStr">
+        <is>
+          <t>1:07:55.879003</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>2020-11-22 091201865016</t>
+        </is>
+      </c>
+      <c r="C494" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>10:19:51.137180</t>
+        </is>
+      </c>
+      <c r="E494" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F494" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G494" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H494" t="n">
+        <v>174000000</v>
+      </c>
+      <c r="I494" t="n">
+        <v>750000</v>
+      </c>
+      <c r="J494" s="5" t="n">
+        <v>44157.38335491917</v>
+      </c>
+      <c r="K494" s="5" t="n">
+        <v>44157.43045297632</v>
+      </c>
+      <c r="L494" t="inlineStr">
+        <is>
+          <t>1:07:49.272138</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>2020-11-22 101958897214</t>
+        </is>
+      </c>
+      <c r="C495" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>11:32:18.676089</t>
+        </is>
+      </c>
+      <c r="E495" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F495" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G495" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H495" t="n">
+        <v>185600000</v>
+      </c>
+      <c r="I495" t="n">
+        <v>800000</v>
+      </c>
+      <c r="J495" s="5" t="n">
+        <v>44157.43054279183</v>
+      </c>
+      <c r="K495" s="5" t="n">
+        <v>44157.48077171369</v>
+      </c>
+      <c r="L495" t="inlineStr">
+        <is>
+          <t>1:12:19.778849</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>2020-11-22 113219959604</t>
+        </is>
+      </c>
+      <c r="C496" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>12:45:04.219787</t>
+        </is>
+      </c>
+      <c r="E496" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F496" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G496" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H496" t="n">
+        <v>185600000</v>
+      </c>
+      <c r="I496" t="n">
+        <v>800000</v>
+      </c>
+      <c r="J496" s="5" t="n">
+        <v>44157.48078656949</v>
+      </c>
+      <c r="K496" s="5" t="n">
+        <v>44157.5312988398</v>
+      </c>
+      <c r="L496" t="inlineStr">
+        <is>
+          <t>1:12:44.260155</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>2020-11-22 124512491494</t>
+        </is>
+      </c>
+      <c r="C497" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>14:02:47.533941</t>
+        </is>
+      </c>
+      <c r="E497" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F497" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G497" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H497" t="n">
+        <v>197200000</v>
+      </c>
+      <c r="I497" t="n">
+        <v>850000</v>
+      </c>
+      <c r="J497" s="5" t="n">
+        <v>44157.53139457749</v>
+      </c>
+      <c r="K497" s="5" t="n">
+        <v>44157.58527238329</v>
+      </c>
+      <c r="L497" t="inlineStr">
+        <is>
+          <t>1:17:35.042422</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>2020-11-22 140248823342</t>
+        </is>
+      </c>
+      <c r="C498" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>15:20:35.382632</t>
+        </is>
+      </c>
+      <c r="E498" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F498" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G498" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H498" t="n">
+        <v>197200000</v>
+      </c>
+      <c r="I498" t="n">
+        <v>850000</v>
+      </c>
+      <c r="J498" s="5" t="n">
+        <v>44157.5852873072</v>
+      </c>
+      <c r="K498" s="5" t="n">
+        <v>44157.63929840978</v>
+      </c>
+      <c r="L498" t="inlineStr">
+        <is>
+          <t>1:17:46.559263</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>2020-11-22 152043920935</t>
+        </is>
+      </c>
+      <c r="C499" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>16:43:01.207157</t>
+        </is>
+      </c>
+      <c r="E499" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F499" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G499" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H499" t="n">
+        <v>208800000</v>
+      </c>
+      <c r="I499" t="n">
+        <v>900000</v>
+      </c>
+      <c r="J499" s="5" t="n">
+        <v>44157.63939723304</v>
+      </c>
+      <c r="K499" s="5" t="n">
+        <v>44157.6965417492</v>
+      </c>
+      <c r="L499" t="inlineStr">
+        <is>
+          <t>1:22:17.286196</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>2020-11-22 164302489440</t>
+        </is>
+      </c>
+      <c r="C500" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D500" t="inlineStr">
+        <is>
+          <t>18:05:24.471869</t>
+        </is>
+      </c>
+      <c r="E500" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F500" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G500" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H500" t="n">
+        <v>208800000</v>
+      </c>
+      <c r="I500" t="n">
+        <v>900000</v>
+      </c>
+      <c r="J500" s="5" t="n">
+        <v>44157.69655659074</v>
+      </c>
+      <c r="K500" s="5" t="n">
+        <v>44157.75375546113</v>
+      </c>
+      <c r="L500" t="inlineStr">
+        <is>
+          <t>1:22:21.982402</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>2020-11-22 180533264024</t>
+        </is>
+      </c>
+      <c r="C501" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>19:32:25.403945</t>
+        </is>
+      </c>
+      <c r="E501" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F501" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G501" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H501" t="n">
+        <v>220400000</v>
+      </c>
+      <c r="I501" t="n">
+        <v>950000</v>
+      </c>
+      <c r="J501" s="5" t="n">
+        <v>44157.7538572225</v>
+      </c>
+      <c r="K501" s="5" t="n">
+        <v>44157.81418291572</v>
+      </c>
+      <c r="L501" t="inlineStr">
+        <is>
+          <t>1:26:52.139894</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>2020-11-22 193226689210</t>
+        </is>
+      </c>
+      <c r="C502" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>20:59:28.217860</t>
+        </is>
+      </c>
+      <c r="E502" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F502" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G502" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H502" t="n">
+        <v>220400000</v>
+      </c>
+      <c r="I502" t="n">
+        <v>950000</v>
+      </c>
+      <c r="J502" s="5" t="n">
+        <v>44157.81419779178</v>
+      </c>
+      <c r="K502" s="5" t="n">
+        <v>44157.87463215082</v>
+      </c>
+      <c r="L502" t="inlineStr">
+        <is>
+          <t>1:27:01.528621</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>2020-11-22 205937314749</t>
+        </is>
+      </c>
+      <c r="C503" s="4" t="n">
+        <v>44157</v>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>22:30:45.538684</t>
+        </is>
+      </c>
+      <c r="E503" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="F503" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="G503" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H503" t="n">
+        <v>232000000</v>
+      </c>
+      <c r="I503" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="J503" s="5" t="n">
+        <v>44157.87473743923</v>
+      </c>
+      <c r="K503" s="5" t="n">
+        <v>44157.9380270677</v>
+      </c>
+      <c r="L503" t="inlineStr">
+        <is>
+          <t>1:31:08.223900</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>2020-11-22 223046879774</t>
+        </is>
+      </c>
+      <c r="C504" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>00:02:10.240391</t>
+        </is>
+      </c>
+      <c r="E504" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F504" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="G504" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="H504" t="n">
+        <v>232000000</v>
+      </c>
+      <c r="I504" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="J504" s="5" t="n">
+        <v>44157.93804258998</v>
+      </c>
+      <c r="K504" s="5" t="n">
+        <v>44158.00150741095</v>
+      </c>
+      <c r="L504" t="inlineStr">
+        <is>
+          <t>1:31:23.360532</t>
         </is>
       </c>
     </row>

</xml_diff>